<commit_message>
Update up to Sprint 3
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16995" windowHeight="11070" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -31,20 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
     <t>Sprint 2</t>
   </si>
   <si>
@@ -138,7 +129,22 @@
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
   </si>
   <si>
-    <t>SUNDEW - AGILE PRODUCT BACKLOG</t>
+    <t xml:space="preserve">SUNDEW - AGILE PRODUCT BACKLOG </t>
+  </si>
+  <si>
+    <t>Design the Login web form.</t>
+  </si>
+  <si>
+    <t>Redesign deployment portfolio</t>
+  </si>
+  <si>
+    <t>Design User Index web form</t>
+  </si>
+  <si>
+    <t>Dsign My Account web form</t>
+  </si>
+  <si>
+    <t>Design User Account web form</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -365,6 +371,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -714,7 +723,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -737,7 +746,7 @@
   <sheetData>
     <row r="1" spans="2:35" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -775,40 +784,40 @@
     </row>
     <row r="2" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -840,30 +849,30 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="6">
         <v>44747</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L3" s="5">
         <f>SUM(L4:L6)</f>
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N3" s="3"/>
       <c r="P3"/>
@@ -888,43 +897,45 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
       <c r="C4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="8">
+        <v>43801</v>
+      </c>
+      <c r="G4" s="8">
+        <v>43802</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="8">
-        <v>44747</v>
-      </c>
-      <c r="G4" s="8">
-        <v>44747</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="7">
-        <v>8</v>
-      </c>
       <c r="M4" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="14"/>
@@ -948,49 +959,51 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
       <c r="C5" s="7" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F5" s="8">
-        <v>44748</v>
+        <v>43803</v>
       </c>
       <c r="G5" s="8">
-        <v>44749</v>
+        <v>43807</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" s="7">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>13</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -1013,48 +1026,26 @@
     </row>
     <row r="6" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="8">
-        <v>44750</v>
-      </c>
-      <c r="G6" s="8">
-        <v>44751</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="3"/>
       <c r="O6" s="15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="15" t="s">
         <v>11</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -1079,7 +1070,7 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
@@ -1088,15 +1079,18 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="L7" s="5">
+        <f>SUM(L8:L10)</f>
+        <v>19</v>
+      </c>
       <c r="M7" s="5"/>
       <c r="N7" s="3"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -1118,18 +1112,42 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="B8" s="20">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="8">
+        <v>43808</v>
+      </c>
+      <c r="G8" s="8">
+        <v>43809</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="20">
+        <v>1</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="N8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -1151,18 +1169,42 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="8">
+        <v>43810</v>
+      </c>
+      <c r="G9" s="8">
+        <v>43811</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="7">
+        <v>5</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1187,18 +1229,42 @@
       <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="B10" s="7">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="8">
+        <v>43812</v>
+      </c>
+      <c r="G10" s="8">
+        <v>43813</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4">
+        <v>13</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -1226,7 +1292,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
@@ -1372,7 +1438,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
@@ -1518,7 +1584,7 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
@@ -1664,7 +1730,7 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
@@ -1810,7 +1876,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -1989,7 +2055,7 @@
     </row>
     <row r="32" spans="2:35" s="12" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -3371,7 +3437,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearrange tasks for sprint 1 and 2
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Design User Account web form</t>
+  </si>
+  <si>
+    <t>Design Main Menu</t>
   </si>
 </sst>
 </file>
@@ -367,13 +370,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -723,7 +726,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -901,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>29</v>
@@ -922,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>12</v>
@@ -963,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>29</v>
@@ -975,7 +978,7 @@
         <v>43803</v>
       </c>
       <c r="G5" s="8">
-        <v>43807</v>
+        <v>43805</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>5</v>
@@ -984,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>12</v>
@@ -1025,16 +1028,36 @@
       <c r="AI5" s="3"/>
     </row>
     <row r="6" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="B6" s="7">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="8">
+        <v>43806</v>
+      </c>
+      <c r="G6" s="8">
+        <v>43807</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="3"/>
@@ -1112,10 +1135,10 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <v>3</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1133,19 +1156,19 @@
       <c r="H8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="18">
         <v>1</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N8" s="3"/>
@@ -1190,10 +1213,10 @@
       <c r="H9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="18" t="s">
         <v>7</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1253,7 +1276,7 @@
       <c r="I10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="18" t="s">
         <v>7</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -1328,7 +1351,6 @@
     </row>
     <row r="12" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
@@ -2054,20 +2076,20 @@
       <c r="AI31" s="3"/>
     </row>
     <row r="32" spans="2:35" s="12" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>

</xml_diff>

<commit_message>
Up to sprint 5, task 13
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="-Disclaimer-" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$J$30</definedName>
     <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$7</definedName>
     <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -93,15 +93,6 @@
     <t>TASK NAME</t>
   </si>
   <si>
-    <t>STORY</t>
-  </si>
-  <si>
-    <t>SPRINT READY</t>
-  </si>
-  <si>
-    <t>ASSIGNED TO SPRINT</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t xml:space="preserve">SUNDEW - AGILE PRODUCT BACKLOG </t>
   </si>
   <si>
-    <t>Design the Login web form.</t>
-  </si>
-  <si>
     <t>Redesign deployment portfolio</t>
   </si>
   <si>
@@ -144,10 +132,31 @@
     <t>Dsign My Account web form</t>
   </si>
   <si>
-    <t>Design User Account web form</t>
-  </si>
-  <si>
     <t>Design Main Menu</t>
+  </si>
+  <si>
+    <t>Design Problems web form</t>
+  </si>
+  <si>
+    <t>Design Jobs web form</t>
+  </si>
+  <si>
+    <t>Design Job Problem web form</t>
+  </si>
+  <si>
+    <t>Design Assign Users web form</t>
+  </si>
+  <si>
+    <t>Implement Boostrap template</t>
+  </si>
+  <si>
+    <t>Design the Login web form</t>
+  </si>
+  <si>
+    <t>Design user account web form</t>
+  </si>
+  <si>
+    <t>Link all forms from main menu</t>
   </si>
 </sst>
 </file>
@@ -725,8 +734,8 @@
   <dimension ref="B1:AI69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -749,7 +758,7 @@
   <sheetData>
     <row r="1" spans="2:35" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -799,29 +808,21 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="K2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -845,38 +846,32 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" s="6">
-        <v>44747</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>44903</v>
+      </c>
+      <c r="G3" s="6">
+        <v>44910</v>
+      </c>
       <c r="H3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="5">
-        <f>SUM(L4:L6)</f>
-        <v>41</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="J3" s="5">
+        <f>SUM(J4:J6)</f>
+        <v>17</v>
+      </c>
+      <c r="K3" s="20"/>
       <c r="N3" s="3"/>
       <c r="P3"/>
       <c r="Q3"/>
@@ -907,38 +902,30 @@
         <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F4" s="8">
-        <v>43801</v>
+        <v>43807</v>
       </c>
       <c r="G4" s="8">
-        <v>43802</v>
+        <v>43808</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J4" s="7">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="14"/>
@@ -969,35 +956,27 @@
         <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F5" s="8">
-        <v>43803</v>
+        <v>43807</v>
       </c>
       <c r="G5" s="8">
-        <v>43805</v>
+        <v>43808</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="7">
-        <v>40</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="15" t="s">
         <v>5</v>
@@ -1032,34 +1011,30 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="8">
-        <v>43806</v>
+        <v>43809</v>
       </c>
       <c r="G6" s="8">
-        <v>43807</v>
+        <v>43810</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="J6" s="7">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="15" t="s">
         <v>6</v>
@@ -1100,13 +1075,11 @@
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5">
-        <f>SUM(L8:L10)</f>
+      <c r="J7" s="5">
+        <f>SUM(J8:J10)</f>
         <v>19</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="K7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15" t="s">
@@ -1135,42 +1108,34 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="18">
-        <v>3</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>35</v>
+      <c r="B8" s="7">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="8">
-        <v>43808</v>
+        <v>43811</v>
       </c>
       <c r="G8" s="8">
-        <v>43809</v>
+        <v>43814</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="18">
-        <v>1</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>5</v>
-      </c>
+      <c r="J8" s="7">
+        <v>13</v>
+      </c>
+      <c r="K8" s="3"/>
       <c r="N8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -1192,42 +1157,34 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>36</v>
+      <c r="B9" s="18">
+        <v>5</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" s="8">
-        <v>43810</v>
+        <v>43815</v>
       </c>
       <c r="G9" s="8">
-        <v>43811</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="18" t="s">
+        <v>43816</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="7">
-        <v>5</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J9" s="18">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1253,41 +1210,33 @@
     </row>
     <row r="10" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="8">
+        <v>43817</v>
+      </c>
+      <c r="G10" s="8">
+        <v>43818</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="7">
         <v>5</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="8">
-        <v>43812</v>
-      </c>
-      <c r="G10" s="8">
-        <v>43813</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="4">
-        <v>13</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="K10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -1322,10 +1271,11 @@
       <c r="G11" s="6"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="J11" s="5">
+        <f>SUM(J12:J14)</f>
+        <v>26</v>
+      </c>
+      <c r="K11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -1350,17 +1300,34 @@
       <c r="AI11" s="3"/>
     </row>
     <row r="12" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="B12" s="7">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="8">
+        <v>43819</v>
+      </c>
+      <c r="G12" s="8">
+        <v>43820</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="7">
+        <v>13</v>
+      </c>
+      <c r="K12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -1385,18 +1352,34 @@
       <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="B13" s="7">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="8">
+        <v>43821</v>
+      </c>
+      <c r="G13" s="8">
+        <v>43822</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="7">
+        <v>5</v>
+      </c>
+      <c r="K13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -1421,18 +1404,34 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="B14" s="7">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="8">
+        <v>43823</v>
+      </c>
+      <c r="G14" s="8">
+        <v>43824</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="7">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -1468,9 +1467,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="K15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -1495,18 +1492,34 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="B16" s="7">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="8">
+        <v>43829</v>
+      </c>
+      <c r="G16" s="8">
+        <v>43830</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="7">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1531,18 +1544,34 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="B17" s="7">
+        <v>10</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="8">
+        <v>43825</v>
+      </c>
+      <c r="G17" s="8">
+        <v>43826</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="7">
+        <v>8</v>
+      </c>
+      <c r="K17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -1567,18 +1596,34 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="B18" s="7">
+        <v>11</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="8">
+        <v>43827</v>
+      </c>
+      <c r="G18" s="8">
+        <v>43828</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="7">
+        <v>13</v>
+      </c>
+      <c r="K18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -1614,9 +1659,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="K19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -1641,18 +1684,34 @@
       <c r="AI19" s="3"/>
     </row>
     <row r="20" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="B20" s="7">
+        <v>12</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="8">
+        <v>43829</v>
+      </c>
+      <c r="G20" s="8">
+        <v>43830</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="7">
+        <v>20</v>
+      </c>
+      <c r="K20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -1677,18 +1736,24 @@
       <c r="AI20" s="3"/>
     </row>
     <row r="21" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
+      <c r="B21" s="7">
+        <v>13</v>
+      </c>
       <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="I21" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="K21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -1715,16 +1780,20 @@
     <row r="22" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
+      <c r="K22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -1752,7 +1821,7 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
@@ -1760,9 +1829,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="K23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -1789,16 +1856,20 @@
     <row r="24" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
+      <c r="K24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -1825,16 +1896,20 @@
     <row r="25" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="K25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -1861,16 +1936,20 @@
     <row r="26" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="I26" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="K26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -1898,7 +1977,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -1906,9 +1985,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="K27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -1935,16 +2012,20 @@
     <row r="28" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="D28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="I28" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="K28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -1971,16 +2052,20 @@
     <row r="29" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+      <c r="D29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="I29" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="K29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -2007,16 +2092,20 @@
     <row r="30" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="I30" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
+      <c r="K30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -2077,17 +2166,17 @@
     </row>
     <row r="32" spans="2:35" s="12" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
       <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
       <c r="N32" s="10"/>
@@ -2399,10 +2488,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
       <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -2434,10 +2520,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
       <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -2469,10 +2552,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
       <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -2504,10 +2584,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
       <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -2539,10 +2616,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
       <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -2574,10 +2648,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -2609,10 +2680,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -2644,10 +2712,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -2679,10 +2744,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -2714,10 +2776,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -2749,10 +2808,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -2784,10 +2840,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
@@ -2819,10 +2872,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
@@ -2854,10 +2904,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
@@ -2889,10 +2936,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -2924,10 +2968,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
@@ -2959,10 +3000,7 @@
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
@@ -2994,10 +3032,7 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
@@ -3029,10 +3064,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
@@ -3064,10 +3096,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
@@ -3099,10 +3128,7 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
@@ -3134,10 +3160,7 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
@@ -3169,10 +3192,7 @@
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
       <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
@@ -3204,10 +3224,7 @@
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
@@ -3239,10 +3256,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
       <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
@@ -3274,10 +3288,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
       <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
@@ -3309,10 +3320,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
       <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
@@ -3344,10 +3352,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
@@ -3379,10 +3384,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
       <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
@@ -3409,17 +3411,11 @@
       <c r="AI69" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B32:M32"/>
-  </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I30 M3:M30">
-      <formula1>YesNo</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J30">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H30">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I30">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6">
@@ -3459,7 +3455,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update up to sprint 8
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="69">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Setup Auth 0</t>
   </si>
   <si>
-    <t>Code the User Index web form</t>
-  </si>
-  <si>
     <t>Design Login</t>
   </si>
   <si>
@@ -223,6 +220,24 @@
   </si>
   <si>
     <t>Sprint 20</t>
+  </si>
+  <si>
+    <t>Implement CreateUser method in NewUserAccount web form</t>
+  </si>
+  <si>
+    <t>Implement ReadUsers method in User Index web form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement UpdateUser method  in User account web form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Delete User method in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement ReadUser method  in User account web form </t>
+  </si>
+  <si>
+    <t>Implement CRUD user functionality</t>
   </si>
 </sst>
 </file>
@@ -790,9 +805,9 @@
   </sheetPr>
   <dimension ref="B1:AI82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -906,7 +921,7 @@
     <row r="3" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
@@ -1126,7 +1141,7 @@
     <row r="7" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>1</v>
@@ -1326,7 +1341,7 @@
     <row r="11" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>2</v>
@@ -1525,7 +1540,7 @@
     <row r="15" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
@@ -1724,7 +1739,7 @@
     <row r="19" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>4</v>
@@ -1923,7 +1938,7 @@
     <row r="23" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>22</v>
@@ -1933,7 +1948,10 @@
       <c r="G23" s="6"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="J23" s="5">
+        <f>SUM(J24:J26)</f>
+        <v>120</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -2015,7 +2033,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>24</v>
@@ -2026,12 +2044,18 @@
       <c r="F25" s="8">
         <v>43843</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="7"/>
+      <c r="G25" s="8">
+        <v>43848</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="7"/>
+      <c r="J25" s="7">
+        <v>40</v>
+      </c>
       <c r="K25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -2057,21 +2081,33 @@
       <c r="AI25" s="3"/>
     </row>
     <row r="26" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="7">
+        <v>17</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="D26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="7"/>
+      <c r="F26" s="8">
+        <v>43849</v>
+      </c>
+      <c r="G26" s="8">
+        <v>43854</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="7"/>
+      <c r="J26" s="7">
+        <v>40</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
@@ -2098,7 +2134,9 @@
     </row>
     <row r="27" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
@@ -2109,7 +2147,10 @@
       <c r="G27" s="6"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
+      <c r="J27" s="5">
+        <f>SUM(J28:J30)</f>
+        <v>120</v>
+      </c>
       <c r="K27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -2135,21 +2176,33 @@
       <c r="AI27" s="3"/>
     </row>
     <row r="28" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="7">
+        <v>18</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="D28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
+      <c r="F28" s="8">
+        <v>43855</v>
+      </c>
+      <c r="G28" s="8">
+        <v>43857</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="7"/>
+      <c r="J28" s="7">
+        <v>40</v>
+      </c>
       <c r="K28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -2175,21 +2228,33 @@
       <c r="AI28" s="3"/>
     </row>
     <row r="29" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="7">
+        <v>19</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="D29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="7"/>
+      <c r="F29" s="8">
+        <v>43858</v>
+      </c>
+      <c r="G29" s="8">
+        <v>43861</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J29" s="7"/>
+      <c r="J29" s="7">
+        <v>40</v>
+      </c>
       <c r="K29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -2215,21 +2280,33 @@
       <c r="AI29" s="3"/>
     </row>
     <row r="30" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="7">
+        <v>20</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="7"/>
+      <c r="F30" s="8">
+        <v>43862</v>
+      </c>
+      <c r="G30" s="8">
+        <v>43866</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="7"/>
+      <c r="J30" s="7">
+        <v>40</v>
+      </c>
       <c r="K30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
@@ -2258,7 +2335,7 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>24</v>
@@ -2267,7 +2344,10 @@
       <c r="G31" s="6"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+      <c r="J31" s="5">
+        <f>SUM(J32:J34)</f>
+        <v>0</v>
+      </c>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
       <c r="M31" s="10"/>
@@ -2423,7 +2503,7 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>24</v>
@@ -2432,7 +2512,10 @@
       <c r="G35" s="6"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
+      <c r="J35" s="5">
+        <f>SUM(J36:J38)</f>
+        <v>0</v>
+      </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -2589,7 +2672,7 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>24</v>
@@ -2598,7 +2681,10 @@
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
+      <c r="J39" s="5">
+        <f>SUM(J40:J42)</f>
+        <v>0</v>
+      </c>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -2752,7 +2838,7 @@
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>24</v>
@@ -2761,7 +2847,10 @@
       <c r="G43" s="6"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
+      <c r="J43" s="5">
+        <f>SUM(J44:J46)</f>
+        <v>0</v>
+      </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -2914,7 +3003,7 @@
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>24</v>
@@ -2923,7 +3012,10 @@
       <c r="G47" s="6"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
+      <c r="J47" s="5">
+        <f>SUM(J48:J50)</f>
+        <v>0</v>
+      </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -3076,7 +3168,7 @@
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>24</v>
@@ -3085,7 +3177,10 @@
       <c r="G51" s="6"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
+      <c r="J51" s="5">
+        <f>SUM(J52:J54)</f>
+        <v>0</v>
+      </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -3238,7 +3333,7 @@
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>24</v>
@@ -3247,7 +3342,10 @@
       <c r="G55" s="6"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
+      <c r="J55" s="5">
+        <f>SUM(J56:J58)</f>
+        <v>0</v>
+      </c>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -3400,7 +3498,7 @@
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>24</v>
@@ -3409,7 +3507,10 @@
       <c r="G59" s="6"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
+      <c r="J59" s="5">
+        <f>SUM(J60:J62)</f>
+        <v>0</v>
+      </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
@@ -3562,7 +3663,7 @@
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>24</v>
@@ -3571,7 +3672,10 @@
       <c r="G63" s="6"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
+      <c r="J63" s="5">
+        <f>SUM(J64:J66)</f>
+        <v>0</v>
+      </c>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
@@ -3724,7 +3828,7 @@
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>24</v>
@@ -3733,7 +3837,10 @@
       <c r="G67" s="6"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
+      <c r="J67" s="5">
+        <f>SUM(J68:J70)</f>
+        <v>0</v>
+      </c>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
@@ -3838,7 +3945,7 @@
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>24</v>
@@ -3847,7 +3954,10 @@
       <c r="G71" s="6"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
+      <c r="J71" s="5">
+        <f>SUM(J72:J74)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
@@ -3904,7 +4014,7 @@
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>24</v>
@@ -3913,7 +4023,10 @@
       <c r="G75" s="6"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
+      <c r="J75" s="5">
+        <f>SUM(J76:J78)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
@@ -3970,7 +4083,7 @@
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>24</v>
@@ -3979,7 +4092,10 @@
       <c r="G79" s="6"/>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
+      <c r="J79" s="5">
+        <f>SUM(J80:J82)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>

</xml_diff>

<commit_message>
Alter incomplete sprint 6 and at sprint 9
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -16,6 +16,8 @@
     <sheet name="-Disclaimer-" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_Toc26117415" localSheetId="0">'Agile Product Backlog'!$C$34</definedName>
+    <definedName name="_Toc26117416" localSheetId="0">'Agile Product Backlog'!$C$36</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$J$30</definedName>
     <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$7</definedName>
     <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="76">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -238,6 +240,27 @@
   </si>
   <si>
     <t>Implement CRUD user functionality</t>
+  </si>
+  <si>
+    <t>Implement User search and verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement SearchUsers method  in User account web form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement VerifyPassword  method  in User account web form </t>
+  </si>
+  <si>
+    <t>Implement ConfirmRequiredContactInfoProvided method  in User account web form</t>
+  </si>
+  <si>
+    <t>2020/02/012</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Implement method Confirm Required Contact Info Provided for User Account web form</t>
   </si>
 </sst>
 </file>
@@ -805,9 +828,9 @@
   </sheetPr>
   <dimension ref="B1:AI82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>24</v>
@@ -1784,7 +1807,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>24</v>
@@ -1799,7 +1822,7 @@
         <v>43830</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>12</v>
@@ -1980,9 +2003,6 @@
       <c r="B24" s="7">
         <v>15</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="D24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2296,7 +2316,7 @@
         <v>43862</v>
       </c>
       <c r="G30" s="8">
-        <v>43866</v>
+        <v>43867</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>7</v>
@@ -2333,7 +2353,9 @@
     </row>
     <row r="31" spans="2:35" s="12" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="D31" s="5" t="s">
         <v>50</v>
       </c>
@@ -2374,17 +2396,27 @@
       <c r="AH31" s="11"/>
     </row>
     <row r="32" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="7">
+        <v>21</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="D32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="7"/>
+      <c r="F32" s="8">
+        <v>43868</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="I32" s="7" t="s">
         <v>12</v>
       </c>
@@ -2416,17 +2448,27 @@
       <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="B33" s="7">
+        <v>22</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="7"/>
+      <c r="F33" s="8">
+        <v>43874</v>
+      </c>
+      <c r="G33" s="8">
+        <v>43878</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="I33" s="7" t="s">
         <v>12</v>
       </c>
@@ -2458,17 +2500,27 @@
       <c r="AI33" s="3"/>
     </row>
     <row r="34" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="B34" s="7">
+        <v>23</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="7"/>
+      <c r="F34" s="8">
+        <v>43879</v>
+      </c>
+      <c r="G34" s="8">
+        <v>43883</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I34" s="7" t="s">
         <v>12</v>
       </c>
@@ -2501,7 +2553,9 @@
     </row>
     <row r="35" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="D35" s="5" t="s">
         <v>51</v>
       </c>
@@ -2543,17 +2597,27 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+      <c r="B36" s="7">
+        <v>24</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="7"/>
+      <c r="F36" s="8">
+        <v>43887</v>
+      </c>
+      <c r="G36" s="8">
+        <v>43890</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I36" s="7" t="s">
         <v>12</v>
       </c>
@@ -2585,7 +2649,9 @@
       <c r="AI36" s="3"/>
     </row>
     <row r="37" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
+      <c r="B37" s="7">
+        <v>25</v>
+      </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
         <v>24</v>
@@ -2627,7 +2693,9 @@
       <c r="AI37" s="3"/>
     </row>
     <row r="38" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
+      <c r="B38" s="7">
+        <v>26</v>
+      </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7" t="s">
         <v>24</v>
@@ -2712,7 +2780,9 @@
       <c r="AI39" s="3"/>
     </row>
     <row r="40" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
+      <c r="B40" s="7">
+        <v>27</v>
+      </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
         <v>24</v>
@@ -2753,7 +2823,9 @@
       <c r="AI40" s="3"/>
     </row>
     <row r="41" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
+      <c r="B41" s="7">
+        <v>28</v>
+      </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update up to Sprint 12
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -18,6 +18,9 @@
   <definedNames>
     <definedName name="_Toc26117415" localSheetId="0">'Agile Product Backlog'!$C$34</definedName>
     <definedName name="_Toc26117416" localSheetId="0">'Agile Product Backlog'!$C$36</definedName>
+    <definedName name="_Toc26117420" localSheetId="0">'Agile Product Backlog'!$C$46</definedName>
+    <definedName name="_Toc26117425" localSheetId="0">'Agile Product Backlog'!$C$45</definedName>
+    <definedName name="_Toc26117426" localSheetId="0">'Agile Product Backlog'!$C$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$J$30</definedName>
     <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$7</definedName>
     <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="86">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -152,9 +155,6 @@
     <t>Design the Login web form</t>
   </si>
   <si>
-    <t>Design user account web form</t>
-  </si>
-  <si>
     <t>Link all forms from main menu</t>
   </si>
   <si>
@@ -257,10 +257,43 @@
     <t>2020/02/012</t>
   </si>
   <si>
-    <t>Registration</t>
-  </si>
-  <si>
-    <t>Implement method Confirm Required Contact Info Provided for User Account web form</t>
+    <t>Brush up on tech used for project.</t>
+  </si>
+  <si>
+    <t>Implement method ConfirmRequired ContactInfoProvided for User Account web form</t>
+  </si>
+  <si>
+    <t>Ensure User system works as per specs</t>
+  </si>
+  <si>
+    <t>Create job system</t>
+  </si>
+  <si>
+    <t>Implement method CreateJob in the Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement method JobStartDate in the Jobs webform</t>
+  </si>
+  <si>
+    <t>Design User account web form</t>
+  </si>
+  <si>
+    <t>Implement CRUD ops for job system</t>
+  </si>
+  <si>
+    <t>Implement user search and verification part 2</t>
+  </si>
+  <si>
+    <t>Implement method ConfirmRequired JobInfoProvided</t>
+  </si>
+  <si>
+    <t>Implement method UpdateJob in the Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement method DeleteJob in the Jobs webform</t>
+  </si>
+  <si>
+    <t>Delete All Job Problems</t>
   </si>
 </sst>
 </file>
@@ -829,8 +862,8 @@
   <dimension ref="B1:AI82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -944,7 +977,7 @@
     <row r="3" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
@@ -956,13 +989,13 @@
         <v>44903</v>
       </c>
       <c r="G3" s="6">
-        <v>44910</v>
+        <v>44906</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" s="5">
         <f>SUM(J4:J6)</f>
@@ -1164,7 +1197,7 @@
     <row r="7" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>1</v>
@@ -1364,7 +1397,7 @@
     <row r="11" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>2</v>
@@ -1409,7 +1442,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>24</v>
@@ -1563,7 +1596,7 @@
     <row r="15" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
@@ -1608,7 +1641,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>24</v>
@@ -1762,7 +1795,7 @@
     <row r="19" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>4</v>
@@ -1807,7 +1840,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>24</v>
@@ -1859,7 +1892,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>24</v>
@@ -1911,7 +1944,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>24</v>
@@ -1961,7 +1994,7 @@
     <row r="23" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>22</v>
@@ -1973,7 +2006,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5">
         <f>SUM(J24:J26)</f>
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="K23" s="3"/>
       <c r="N23" s="3"/>
@@ -2003,6 +2036,9 @@
       <c r="B24" s="7">
         <v>15</v>
       </c>
+      <c r="C24" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="D24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2016,13 +2052,13 @@
         <v>43842</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J24" s="7">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="K24" s="3"/>
       <c r="N24" s="3"/>
@@ -2053,7 +2089,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>24</v>
@@ -2105,7 +2141,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>24</v>
@@ -2155,7 +2191,7 @@
     <row r="27" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
@@ -2199,8 +2235,8 @@
       <c r="B28" s="7">
         <v>18</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>67</v>
+      <c r="C28" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>24</v>
@@ -2254,7 +2290,7 @@
       <c r="C29" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -2304,7 +2340,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>24</v>
@@ -2354,10 +2390,10 @@
     <row r="31" spans="2:35" s="12" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>24</v>
@@ -2368,7 +2404,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5">
         <f>SUM(J32:J34)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
@@ -2400,7 +2436,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>24</v>
@@ -2412,7 +2448,7 @@
         <v>43868</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>9</v>
@@ -2420,7 +2456,9 @@
       <c r="I32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="7"/>
+      <c r="J32" s="7">
+        <v>2</v>
+      </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2452,7 +2490,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
@@ -2472,7 +2510,9 @@
       <c r="I33" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J33" s="7"/>
+      <c r="J33" s="7">
+        <v>5</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2504,7 +2544,7 @@
         <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>24</v>
@@ -2524,7 +2564,9 @@
       <c r="I34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="7"/>
+      <c r="J34" s="7">
+        <v>40</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2554,10 +2596,10 @@
     <row r="35" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>24</v>
@@ -2568,7 +2610,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5">
         <f>SUM(J36:J38)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -2601,7 +2643,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>24</v>
@@ -2621,7 +2663,9 @@
       <c r="I36" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="7"/>
+      <c r="J36" s="7">
+        <v>40</v>
+      </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -2652,20 +2696,30 @@
       <c r="B37" s="7">
         <v>25</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="7"/>
+      <c r="F37" s="8">
+        <v>43891</v>
+      </c>
+      <c r="G37" s="8">
+        <v>43897</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I37" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="7"/>
+      <c r="J37" s="7">
+        <v>40</v>
+      </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -2693,10 +2747,7 @@
       <c r="AI37" s="3"/>
     </row>
     <row r="38" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
-        <v>26</v>
-      </c>
-      <c r="C38" s="7"/>
+      <c r="B38" s="7"/>
       <c r="D38" s="7" t="s">
         <v>24</v>
       </c>
@@ -2706,9 +2757,7 @@
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -2738,9 +2787,11 @@
     </row>
     <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="D39" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>24</v>
@@ -2751,7 +2802,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5">
         <f>SUM(J40:J42)</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -2781,22 +2832,32 @@
     </row>
     <row r="40" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7">
-        <v>27</v>
-      </c>
-      <c r="C40" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="7"/>
+      <c r="F40" s="8">
+        <v>43898</v>
+      </c>
+      <c r="G40" s="8">
+        <v>43905</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="I40" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="7"/>
+      <c r="J40" s="7">
+        <v>1</v>
+      </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -2824,22 +2885,32 @@
     </row>
     <row r="41" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7">
-        <v>28</v>
-      </c>
-      <c r="C41" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="7"/>
+      <c r="F41" s="8">
+        <v>43906</v>
+      </c>
+      <c r="G41" s="8">
+        <v>43908</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I41" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J41" s="7"/>
+      <c r="J41" s="7">
+        <v>40</v>
+      </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -2866,21 +2937,33 @@
       <c r="AI41" s="3"/>
     </row>
     <row r="42" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="B42" s="7">
+        <v>28</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
+      <c r="F42" s="8">
+        <v>43909</v>
+      </c>
+      <c r="G42" s="8">
+        <v>43913</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J42" s="7"/>
+      <c r="J42" s="7">
+        <v>40</v>
+      </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -2908,9 +2991,11 @@
     </row>
     <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D43" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>24</v>
@@ -2921,7 +3006,7 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5">
         <f>SUM(J44:J46)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -2949,21 +3034,33 @@
       <c r="AI43" s="3"/>
     </row>
     <row r="44" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+      <c r="B44" s="7">
+        <v>29</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="7"/>
+      <c r="F44" s="8">
+        <v>43914</v>
+      </c>
+      <c r="G44" s="8">
+        <v>43917</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I44" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="7"/>
+      <c r="J44" s="7">
+        <v>13</v>
+      </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -2990,21 +3087,33 @@
       <c r="AI44" s="3"/>
     </row>
     <row r="45" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+      <c r="B45" s="7">
+        <v>30</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D45" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="7"/>
+      <c r="F45" s="8">
+        <v>43918</v>
+      </c>
+      <c r="G45" s="8">
+        <v>43921</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="I45" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J45" s="7"/>
+      <c r="J45" s="7">
+        <v>5</v>
+      </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -3031,21 +3140,33 @@
       <c r="AI45" s="3"/>
     </row>
     <row r="46" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+      <c r="B46" s="7">
+        <v>31</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="7"/>
+      <c r="F46" s="8">
+        <v>43922</v>
+      </c>
+      <c r="G46" s="8">
+        <v>43927</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I46" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J46" s="7"/>
+      <c r="J46" s="7">
+        <v>20</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -3075,7 +3196,7 @@
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>24</v>
@@ -3240,7 +3361,7 @@
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>24</v>
@@ -3405,7 +3526,7 @@
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>24</v>
@@ -3570,7 +3691,7 @@
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>24</v>
@@ -3735,7 +3856,7 @@
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>24</v>
@@ -3900,7 +4021,7 @@
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>24</v>
@@ -4017,7 +4138,7 @@
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>24</v>
@@ -4086,7 +4207,7 @@
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>24</v>
@@ -4155,7 +4276,7 @@
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update up to sprint 18
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="110">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -251,9 +251,6 @@
     <t xml:space="preserve">Implement VerifyPassword  method  in User account web form </t>
   </si>
   <si>
-    <t>Implement ConfirmRequiredContactInfoProvided method  in User account web form</t>
-  </si>
-  <si>
     <t>2020/02/012</t>
   </si>
   <si>
@@ -293,7 +290,82 @@
     <t>Implement method DeleteJob in the Jobs webform</t>
   </si>
   <si>
-    <t>Delete All Job Problems</t>
+    <t>Implement CRUD ops for job system part 2</t>
+  </si>
+  <si>
+    <t>2020/</t>
+  </si>
+  <si>
+    <t>Impement ReadJobs in Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement SearchJobs in Job webform</t>
+  </si>
+  <si>
+    <t>Assigning user to job</t>
+  </si>
+  <si>
+    <t>Implement search and TimeDate insertion for job system part 2</t>
+  </si>
+  <si>
+    <t>Implement CRUD ops for problem system</t>
+  </si>
+  <si>
+    <t>Implement DeleteAllJobChats in Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement ReadJob in Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement CreateProblem in Assign Jobs Problem webform</t>
+  </si>
+  <si>
+    <t>Implement UpdateProblem method in Jobs Problem webform</t>
+  </si>
+  <si>
+    <t>Implement reading and searching for problem system</t>
+  </si>
+  <si>
+    <t>Implement DeleteProblem method in Jobs Problem webform</t>
+  </si>
+  <si>
+    <t>Implement ReadProblem method in Jobs Problem webform</t>
+  </si>
+  <si>
+    <t>Implement ReadProblems method in Jobs Problem webform</t>
+  </si>
+  <si>
+    <t>Implement SearchProblems method in jobs webform</t>
+  </si>
+  <si>
+    <t>Implement Attach_zip_file method in Job Problem page</t>
+  </si>
+  <si>
+    <t>Implement Confirm_required_job_info_provided method  in Job web form</t>
+  </si>
+  <si>
+    <t>Implement Confirm_required_contact_info_provided method  in User account web form</t>
+  </si>
+  <si>
+    <t>Implement method Delete_All_Job_Problems in Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement Delete_All_Job_Problems in Jobs webform</t>
+  </si>
+  <si>
+    <t>Implement Auto_Insert_Job_Start_Date webform</t>
+  </si>
+  <si>
+    <t>Implement Register_User_For_Job method in Assign Users webform</t>
+  </si>
+  <si>
+    <t>Implement Confirm Confirm_required_problem_info_provided method in Job webform</t>
+  </si>
+  <si>
+    <t>Implement  Convert_problem_severity_to_text method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement Attach_zip_folder method in Job Problem webform</t>
   </si>
 </sst>
 </file>
@@ -859,11 +931,11 @@
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI82"/>
+  <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1442,7 +1514,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>24</v>
@@ -2037,7 +2109,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>24</v>
@@ -2448,7 +2520,7 @@
         <v>43868</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>9</v>
@@ -2490,7 +2562,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
@@ -2596,7 +2668,7 @@
     <row r="35" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>50</v>
@@ -2643,7 +2715,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>24</v>
@@ -2697,7 +2769,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>24</v>
@@ -2788,7 +2860,7 @@
     <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>51</v>
@@ -2835,7 +2907,7 @@
         <v>26</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>24</v>
@@ -2888,7 +2960,7 @@
         <v>27</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>24</v>
@@ -2941,7 +3013,7 @@
         <v>28</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>24</v>
@@ -2992,7 +3064,7 @@
     <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>52</v>
@@ -3038,7 +3110,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>24</v>
@@ -3091,7 +3163,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>24</v>
@@ -3144,7 +3216,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>24</v>
@@ -3194,7 +3266,9 @@
     </row>
     <row r="47" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="D47" s="5" t="s">
         <v>53</v>
       </c>
@@ -3235,15 +3309,21 @@
       <c r="AI47" s="3"/>
     </row>
     <row r="48" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="B48" s="7">
+        <v>32</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F48" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="G48" s="8"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7" t="s">
@@ -3276,8 +3356,12 @@
       <c r="AI48" s="3"/>
     </row>
     <row r="49" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
+      <c r="B49" s="7">
+        <v>33</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="D49" s="7" t="s">
         <v>24</v>
       </c>
@@ -3317,8 +3401,12 @@
       <c r="AI49" s="3"/>
     </row>
     <row r="50" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="B50" s="7">
+        <v>34</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="D50" s="7" t="s">
         <v>24</v>
       </c>
@@ -3359,7 +3447,9 @@
     </row>
     <row r="51" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="D51" s="5" t="s">
         <v>54</v>
       </c>
@@ -3400,8 +3490,12 @@
       <c r="AI51" s="3"/>
     </row>
     <row r="52" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
+      <c r="B52" s="7">
+        <v>35</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="D52" s="7" t="s">
         <v>24</v>
       </c>
@@ -3441,8 +3535,12 @@
       <c r="AI52" s="3"/>
     </row>
     <row r="53" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
+      <c r="B53" s="7">
+        <v>36</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="D53" s="7" t="s">
         <v>24</v>
       </c>
@@ -3482,8 +3580,12 @@
       <c r="AI53" s="3"/>
     </row>
     <row r="54" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+      <c r="B54" s="7">
+        <v>37</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="D54" s="7" t="s">
         <v>24</v>
       </c>
@@ -3524,7 +3626,9 @@
     </row>
     <row r="55" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+      <c r="C55" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="D55" s="5" t="s">
         <v>55</v>
       </c>
@@ -3565,8 +3669,12 @@
       <c r="AI55" s="3"/>
     </row>
     <row r="56" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
+      <c r="B56" s="7">
+        <v>38</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="D56" s="7" t="s">
         <v>24</v>
       </c>
@@ -3606,8 +3714,12 @@
       <c r="AI56" s="3"/>
     </row>
     <row r="57" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
+      <c r="B57" s="7">
+        <v>39</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="D57" s="7" t="s">
         <v>24</v>
       </c>
@@ -3648,7 +3760,6 @@
     </row>
     <row r="58" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
       <c r="D58" s="7" t="s">
         <v>24</v>
       </c>
@@ -3689,7 +3800,9 @@
     </row>
     <row r="59" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="D59" s="5" t="s">
         <v>56</v>
       </c>
@@ -3730,8 +3843,12 @@
       <c r="AI59" s="3"/>
     </row>
     <row r="60" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="B60" s="7">
+        <v>40</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="D60" s="7" t="s">
         <v>24</v>
       </c>
@@ -3771,8 +3888,12 @@
       <c r="AI60" s="3"/>
     </row>
     <row r="61" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
+      <c r="B61" s="7">
+        <v>41</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>94</v>
+      </c>
       <c r="D61" s="7" t="s">
         <v>24</v>
       </c>
@@ -3812,8 +3933,12 @@
       <c r="AI61" s="3"/>
     </row>
     <row r="62" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+      <c r="B62" s="7">
+        <v>42</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="D62" s="7" t="s">
         <v>24</v>
       </c>
@@ -3854,7 +3979,9 @@
     </row>
     <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="D63" s="5" t="s">
         <v>57</v>
       </c>
@@ -3895,8 +4022,12 @@
       <c r="AI63" s="3"/>
     </row>
     <row r="64" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
+      <c r="B64" s="7">
+        <v>43</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="D64" s="7" t="s">
         <v>24</v>
       </c>
@@ -3936,8 +4067,12 @@
       <c r="AI64" s="3"/>
     </row>
     <row r="65" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
+      <c r="B65" s="7">
+        <v>44</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="D65" s="7" t="s">
         <v>24</v>
       </c>
@@ -3977,8 +4112,12 @@
       <c r="AI65" s="3"/>
     </row>
     <row r="66" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
+      <c r="B66" s="7">
+        <v>45</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="D66" s="7" t="s">
         <v>24</v>
       </c>
@@ -4060,8 +4199,12 @@
       <c r="AI67" s="3"/>
     </row>
     <row r="68" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
+      <c r="B68" s="7">
+        <v>46</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="D68" s="7" t="s">
         <v>24</v>
       </c>
@@ -4101,8 +4244,12 @@
       <c r="AI68" s="3"/>
     </row>
     <row r="69" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
+      <c r="B69" s="7">
+        <v>47</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="D69" s="7" t="s">
         <v>24</v>
       </c>
@@ -4118,8 +4265,12 @@
       <c r="J69" s="7"/>
     </row>
     <row r="70" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
+      <c r="B70" s="7">
+        <v>48</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="D70" s="7" t="s">
         <v>24</v>
       </c>
@@ -4153,8 +4304,12 @@
       </c>
     </row>
     <row r="72" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
+      <c r="B72" s="7">
+        <v>49</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="D72" s="7" t="s">
         <v>24</v>
       </c>
@@ -4341,12 +4496,426 @@
       </c>
       <c r="J82" s="7"/>
     </row>
+    <row r="83" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5">
+        <f>SUM(J84:J86)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J84" s="7"/>
+    </row>
+    <row r="85" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J85" s="7"/>
+    </row>
+    <row r="86" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J86" s="7"/>
+    </row>
+    <row r="87" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5">
+        <f>SUM(J88:J90)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J88" s="7"/>
+    </row>
+    <row r="89" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J89" s="7"/>
+    </row>
+    <row r="90" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J90" s="7"/>
+    </row>
+    <row r="91" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5">
+        <f>SUM(J92:J94)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J93" s="7"/>
+    </row>
+    <row r="94" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J94" s="7"/>
+    </row>
+    <row r="95" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5">
+        <f>SUM(J96:J98)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J96" s="7"/>
+    </row>
+    <row r="97" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J98" s="7"/>
+    </row>
+    <row r="99" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5">
+        <f>SUM(J100:J102)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J101" s="7"/>
+    </row>
+    <row r="102" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J102" s="7"/>
+    </row>
+    <row r="103" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5">
+        <f>SUM(J104:J106)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="7"/>
+    </row>
+    <row r="105" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J105" s="7"/>
+    </row>
+    <row r="106" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J106" s="7"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H82">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H106">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I82">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I106">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6">

</xml_diff>

<commit_message>
Update up to sprint 22
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="131">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Implement search and TimeDate insertion for job system part 2</t>
   </si>
   <si>
-    <t>Implement CRUD ops for problem system</t>
-  </si>
-  <si>
     <t>Implement DeleteAllJobChats in Jobs webform</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>Implement SearchProblems method in jobs webform</t>
   </si>
   <si>
-    <t>Implement Attach_zip_file method in Job Problem page</t>
-  </si>
-  <si>
     <t>Implement Confirm_required_job_info_provided method  in Job web form</t>
   </si>
   <si>
@@ -359,13 +353,82 @@
     <t>Implement Register_User_For_Job method in Assign Users webform</t>
   </si>
   <si>
-    <t>Implement Confirm Confirm_required_problem_info_provided method in Job webform</t>
-  </si>
-  <si>
     <t>Implement  Convert_problem_severity_to_text method in Job Problem webform</t>
   </si>
   <si>
     <t>Implement Attach_zip_folder method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement Confirm_required_problem_info_provided method in Job webform</t>
+  </si>
+  <si>
+    <t>Validate required job data convert problem serverity to text</t>
+  </si>
+  <si>
+    <t>Implement Attachment uploads for problem and perform Chat CRUD ops</t>
+  </si>
+  <si>
+    <t>Implement Chat CRUD ops</t>
+  </si>
+  <si>
+    <t>Implement CreateChat method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement Attach_zip_file method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement Publish_chat_time_and_date method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement ReadChats method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement UpdateChat method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement Chat CRUD ops and validate required data</t>
+  </si>
+  <si>
+    <t>Implement DeleteChat method in Job Problem webform</t>
+  </si>
+  <si>
+    <t>Implement Confirm_required_info_is_not_empty method in JobProblem webform</t>
+  </si>
+  <si>
+    <t>Sprint 22</t>
+  </si>
+  <si>
+    <t>Sprint 21</t>
+  </si>
+  <si>
+    <t>Sprint 23</t>
+  </si>
+  <si>
+    <t>Sprint 24</t>
+  </si>
+  <si>
+    <t>Sprint 25</t>
+  </si>
+  <si>
+    <t>Sprint 26</t>
+  </si>
+  <si>
+    <t>Create problem system</t>
+  </si>
+  <si>
+    <t>Test application</t>
+  </si>
+  <si>
+    <t>Input sample data into app.</t>
+  </si>
+  <si>
+    <t>Create release and create database and reset all primary keys to zero</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Package app into zip</t>
   </si>
 </sst>
 </file>
@@ -934,8 +997,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2562,7 +2625,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
@@ -3216,7 +3279,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>24</v>
@@ -3313,7 +3376,7 @@
         <v>32</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>24</v>
@@ -3360,7 +3423,7 @@
         <v>33</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>24</v>
@@ -3405,7 +3468,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>24</v>
@@ -3584,7 +3647,7 @@
         <v>37</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>24</v>
@@ -3673,7 +3736,7 @@
         <v>38</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>24</v>
@@ -3718,7 +3781,7 @@
         <v>39</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>24</v>
@@ -3801,7 +3864,7 @@
     <row r="59" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>56</v>
@@ -3847,7 +3910,7 @@
         <v>40</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>24</v>
@@ -3892,7 +3955,7 @@
         <v>41</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>24</v>
@@ -3937,7 +4000,7 @@
         <v>42</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>24</v>
@@ -3980,7 +4043,7 @@
     <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>57</v>
@@ -4026,7 +4089,7 @@
         <v>43</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>24</v>
@@ -4071,7 +4134,7 @@
         <v>44</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>24</v>
@@ -4116,7 +4179,7 @@
         <v>45</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>24</v>
@@ -4158,7 +4221,9 @@
     </row>
     <row r="67" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D67" s="5" t="s">
         <v>58</v>
       </c>
@@ -4248,7 +4313,7 @@
         <v>47</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>24</v>
@@ -4265,12 +4330,8 @@
       <c r="J69" s="7"/>
     </row>
     <row r="70" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="7">
-        <v>48</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
       <c r="D70" s="7" t="s">
         <v>24</v>
       </c>
@@ -4287,7 +4348,9 @@
     </row>
     <row r="71" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="D71" s="5" t="s">
         <v>59</v>
       </c>
@@ -4305,10 +4368,10 @@
     </row>
     <row r="72" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>24</v>
@@ -4325,8 +4388,12 @@
       <c r="J72" s="7"/>
     </row>
     <row r="73" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
+      <c r="B73" s="7">
+        <v>49</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="D73" s="7" t="s">
         <v>24</v>
       </c>
@@ -4342,8 +4409,12 @@
       <c r="J73" s="7"/>
     </row>
     <row r="74" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
+      <c r="B74" s="7">
+        <v>50</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="D74" s="7" t="s">
         <v>24</v>
       </c>
@@ -4360,7 +4431,9 @@
     </row>
     <row r="75" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="D75" s="5" t="s">
         <v>60</v>
       </c>
@@ -4377,8 +4450,12 @@
       </c>
     </row>
     <row r="76" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
+      <c r="B76" s="7">
+        <v>51</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="D76" s="7" t="s">
         <v>24</v>
       </c>
@@ -4394,8 +4471,12 @@
       <c r="J76" s="7"/>
     </row>
     <row r="77" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
+      <c r="B77" s="7">
+        <v>52</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="D77" s="7" t="s">
         <v>24</v>
       </c>
@@ -4411,8 +4492,12 @@
       <c r="J77" s="7"/>
     </row>
     <row r="78" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
+      <c r="B78" s="7">
+        <v>53</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="D78" s="7" t="s">
         <v>24</v>
       </c>
@@ -4429,7 +4514,9 @@
     </row>
     <row r="79" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="D79" s="5" t="s">
         <v>61</v>
       </c>
@@ -4446,8 +4533,12 @@
       </c>
     </row>
     <row r="80" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
+      <c r="B80" s="7">
+        <v>54</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="D80" s="7" t="s">
         <v>24</v>
       </c>
@@ -4463,8 +4554,12 @@
       <c r="J80" s="7"/>
     </row>
     <row r="81" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+      <c r="B81" s="7">
+        <v>55</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="D81" s="7" t="s">
         <v>24</v>
       </c>
@@ -4498,9 +4593,11 @@
     </row>
     <row r="83" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="D83" s="5" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>24</v>
@@ -4515,8 +4612,12 @@
       </c>
     </row>
     <row r="84" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
+      <c r="B84" s="7">
+        <v>56</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="D84" s="7" t="s">
         <v>24</v>
       </c>
@@ -4532,8 +4633,12 @@
       <c r="J84" s="7"/>
     </row>
     <row r="85" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
+      <c r="B85" s="7">
+        <v>57</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="D85" s="7" t="s">
         <v>24</v>
       </c>
@@ -4567,9 +4672,11 @@
     </row>
     <row r="87" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
+      <c r="C87" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="D87" s="5" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>24</v>
@@ -4584,8 +4691,12 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
+      <c r="B88" s="7">
+        <v>58</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="D88" s="7" t="s">
         <v>24</v>
       </c>
@@ -4601,7 +4712,9 @@
       <c r="J88" s="7"/>
     </row>
     <row r="89" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="7"/>
+      <c r="B89" s="7">
+        <v>59</v>
+      </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7" t="s">
         <v>24</v>
@@ -4638,7 +4751,7 @@
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>24</v>
@@ -4707,7 +4820,7 @@
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>24</v>
@@ -4776,7 +4889,7 @@
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>24</v>
@@ -4845,7 +4958,7 @@
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update dates and compact workload
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -35,8 +35,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jordan</author>
+  </authors>
+  <commentList>
+    <comment ref="B35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jordan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Up to here.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="132">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -233,9 +268,6 @@
     <t xml:space="preserve">Implement UpdateUser method  in User account web form </t>
   </si>
   <si>
-    <t xml:space="preserve">Implement Delete User method in </t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement ReadUser method  in User account web form </t>
   </si>
   <si>
@@ -251,9 +283,6 @@
     <t xml:space="preserve">Implement VerifyPassword  method  in User account web form </t>
   </si>
   <si>
-    <t>2020/02/012</t>
-  </si>
-  <si>
     <t>Implement method ConfirmRequired ContactInfoProvided for User Account web form</t>
   </si>
   <si>
@@ -429,9 +458,6 @@
   </si>
   <si>
     <t>Show to bussiness owners</t>
-  </si>
-  <si>
-    <t>Upgrade development machine from Windows 7 to 10.</t>
   </si>
   <si>
     <t>2020/06/31</t>
@@ -447,7 +473,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -508,6 +534,19 @@
       <sz val="22"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1001,7 +1040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1009,15 +1048,17 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.25" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="4" customWidth="1"/>
-    <col min="3" max="5" width="33.25" style="4" customWidth="1"/>
+    <col min="3" max="3" width="33.25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.75" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="13.75" style="4" customWidth="1"/>
@@ -1133,10 +1174,10 @@
         <v>33</v>
       </c>
       <c r="F3" s="6">
-        <v>44911</v>
+        <v>43871</v>
       </c>
       <c r="G3" s="6">
-        <v>44916</v>
+        <v>43875</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>7</v>
@@ -1185,10 +1226,10 @@
         <v>24</v>
       </c>
       <c r="F4" s="8">
-        <v>43815</v>
+        <v>43871</v>
       </c>
       <c r="G4" s="8">
-        <v>43816</v>
+        <v>43872</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>9</v>
@@ -1239,10 +1280,10 @@
         <v>24</v>
       </c>
       <c r="F5" s="8">
-        <v>43817</v>
+        <v>43873</v>
       </c>
       <c r="G5" s="8">
-        <v>43818</v>
+        <v>43874</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>9</v>
@@ -1297,10 +1338,10 @@
         <v>24</v>
       </c>
       <c r="F6" s="8">
-        <v>43819</v>
+        <v>43875</v>
       </c>
       <c r="G6" s="8">
-        <v>43820</v>
+        <v>43875</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>7</v>
@@ -1353,10 +1394,10 @@
         <v>24</v>
       </c>
       <c r="F7" s="6">
-        <v>43821</v>
+        <v>43877</v>
       </c>
       <c r="G7" s="6">
-        <v>43828</v>
+        <v>43882</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>7</v>
@@ -1410,10 +1451,10 @@
         <v>24</v>
       </c>
       <c r="F8" s="8">
-        <v>43821</v>
+        <v>43877</v>
       </c>
       <c r="G8" s="8">
-        <v>43824</v>
+        <v>43878</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>7</v>
@@ -1459,10 +1500,10 @@
         <v>24</v>
       </c>
       <c r="F9" s="8">
-        <v>43825</v>
+        <v>43879</v>
       </c>
       <c r="G9" s="8">
-        <v>43826</v>
+        <v>43880</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>7</v>
@@ -1511,10 +1552,10 @@
         <v>24</v>
       </c>
       <c r="F10" s="8">
-        <v>43827</v>
+        <v>43881</v>
       </c>
       <c r="G10" s="8">
-        <v>43828</v>
+        <v>43882</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>7</v>
@@ -1561,7 +1602,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="6">
-        <v>43829</v>
+        <v>43883</v>
       </c>
       <c r="G11" s="6">
         <v>43841</v>
@@ -1605,7 +1646,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>24</v>
@@ -1614,10 +1655,10 @@
         <v>24</v>
       </c>
       <c r="F12" s="8">
-        <v>43829</v>
+        <v>43884</v>
       </c>
       <c r="G12" s="8">
-        <v>43830</v>
+        <v>43885</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>7</v>
@@ -1666,10 +1707,10 @@
         <v>24</v>
       </c>
       <c r="F13" s="8">
-        <v>43831</v>
+        <v>43886</v>
       </c>
       <c r="G13" s="8">
-        <v>43839</v>
+        <v>43887</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>8</v>
@@ -1718,10 +1759,10 @@
         <v>24</v>
       </c>
       <c r="F14" s="8">
-        <v>43840</v>
+        <v>43888</v>
       </c>
       <c r="G14" s="8">
-        <v>43841</v>
+        <v>43889</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>8</v>
@@ -1768,10 +1809,10 @@
         <v>24</v>
       </c>
       <c r="F15" s="6">
-        <v>43842</v>
+        <v>43891</v>
       </c>
       <c r="G15" s="6">
-        <v>43850</v>
+        <v>43896</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>7</v>
@@ -1821,10 +1862,10 @@
         <v>24</v>
       </c>
       <c r="F16" s="8">
-        <v>43842</v>
+        <v>43891</v>
       </c>
       <c r="G16" s="8">
-        <v>43846</v>
+        <v>43892</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>8</v>
@@ -1873,10 +1914,10 @@
         <v>24</v>
       </c>
       <c r="F17" s="8">
-        <v>43847</v>
+        <v>43893</v>
       </c>
       <c r="G17" s="8">
-        <v>43848</v>
+        <v>43894</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>7</v>
@@ -1925,10 +1966,10 @@
         <v>24</v>
       </c>
       <c r="F18" s="8">
-        <v>43849</v>
+        <v>43895</v>
       </c>
       <c r="G18" s="8">
-        <v>43850</v>
+        <v>43896</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>7</v>
@@ -1975,7 +2016,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="6">
-        <v>43851</v>
+        <v>43898</v>
       </c>
       <c r="G19" s="6">
         <v>43860</v>
@@ -2028,10 +2069,10 @@
         <v>24</v>
       </c>
       <c r="F20" s="8">
-        <v>43851</v>
+        <v>43899</v>
       </c>
       <c r="G20" s="8">
-        <v>43855</v>
+        <v>43900</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>8</v>
@@ -2080,10 +2121,10 @@
         <v>24</v>
       </c>
       <c r="F21" s="8">
-        <v>43856</v>
+        <v>43901</v>
       </c>
       <c r="G21" s="8">
-        <v>43858</v>
+        <v>43904</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>7</v>
@@ -2132,10 +2173,10 @@
         <v>24</v>
       </c>
       <c r="F22" s="8">
-        <v>43859</v>
+        <v>43906</v>
       </c>
       <c r="G22" s="8">
-        <v>43860</v>
+        <v>43908</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>7</v>
@@ -2182,10 +2223,10 @@
         <v>24</v>
       </c>
       <c r="F23" s="6">
-        <v>43861</v>
+        <v>43910</v>
       </c>
       <c r="G23" s="6">
-        <v>43854</v>
+        <v>43912</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>8</v>
@@ -2195,7 +2236,7 @@
       </c>
       <c r="J23" s="5">
         <f>SUM(J24:J26)</f>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K23" s="3"/>
       <c r="N23" s="3"/>
@@ -2222,33 +2263,14 @@
       <c r="AI23" s="3"/>
     </row>
     <row r="24" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
-        <v>15</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="8">
-        <v>43861</v>
-      </c>
-      <c r="G24" s="8">
-        <v>43864</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="7">
-        <v>2</v>
-      </c>
+      <c r="B24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2287,10 +2309,10 @@
         <v>24</v>
       </c>
       <c r="F25" s="8">
-        <v>43843</v>
+        <v>43910</v>
       </c>
       <c r="G25" s="8">
-        <v>43848</v>
+        <v>43913</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>7</v>
@@ -2339,10 +2361,10 @@
         <v>24</v>
       </c>
       <c r="F26" s="8">
-        <v>43849</v>
+        <v>43917</v>
       </c>
       <c r="G26" s="8">
-        <v>43854</v>
+        <v>43922</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>7</v>
@@ -2380,7 +2402,7 @@
     <row r="27" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
@@ -2389,10 +2411,10 @@
         <v>24</v>
       </c>
       <c r="F27" s="6">
-        <v>43855</v>
+        <v>43922</v>
       </c>
       <c r="G27" s="6">
-        <v>43867</v>
+        <v>43924</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>7</v>
@@ -2402,7 +2424,7 @@
       </c>
       <c r="J27" s="5">
         <f>SUM(J28:J30)</f>
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="K27" s="3"/>
       <c r="N27" s="3"/>
@@ -2429,33 +2451,15 @@
       <c r="AI27" s="3"/>
     </row>
     <row r="28" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
-        <v>18</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="8">
-        <v>43855</v>
-      </c>
-      <c r="G28" s="8">
-        <v>43857</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="7">
-        <v>40</v>
-      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
       <c r="K28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -2485,7 +2489,7 @@
         <v>19</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>24</v>
@@ -2494,10 +2498,10 @@
         <v>24</v>
       </c>
       <c r="F29" s="8">
-        <v>43858</v>
+        <v>43925</v>
       </c>
       <c r="G29" s="8">
-        <v>43861</v>
+        <v>43927</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>7</v>
@@ -2546,10 +2550,10 @@
         <v>24</v>
       </c>
       <c r="F30" s="8">
-        <v>43862</v>
+        <v>43927</v>
       </c>
       <c r="G30" s="8">
-        <v>43867</v>
+        <v>43929</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>7</v>
@@ -2587,7 +2591,7 @@
     <row r="31" spans="2:35" s="12" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>49</v>
@@ -2596,10 +2600,10 @@
         <v>24</v>
       </c>
       <c r="F31" s="6">
-        <v>43868</v>
+        <v>43929</v>
       </c>
       <c r="G31" s="6">
-        <v>43883</v>
+        <v>43871</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>9</v>
@@ -2641,7 +2645,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>24</v>
@@ -2650,10 +2654,10 @@
         <v>24</v>
       </c>
       <c r="F32" s="8">
-        <v>43868</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>71</v>
+        <v>43929</v>
+      </c>
+      <c r="G32" s="8">
+        <v>43931</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>9</v>
@@ -2695,7 +2699,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
@@ -2704,10 +2708,10 @@
         <v>24</v>
       </c>
       <c r="F33" s="8">
-        <v>43874</v>
+        <v>43934</v>
       </c>
       <c r="G33" s="8">
-        <v>43878</v>
+        <v>43937</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>8</v>
@@ -2749,7 +2753,7 @@
         <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>24</v>
@@ -2758,10 +2762,10 @@
         <v>24</v>
       </c>
       <c r="F34" s="8">
-        <v>43879</v>
+        <v>43938</v>
       </c>
       <c r="G34" s="8">
-        <v>43883</v>
+        <v>43940</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>7</v>
@@ -2801,7 +2805,7 @@
     <row r="35" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>50</v>
@@ -2810,7 +2814,7 @@
         <v>24</v>
       </c>
       <c r="F35" s="6">
-        <v>43887</v>
+        <v>43886</v>
       </c>
       <c r="G35" s="6">
         <v>43897</v>
@@ -2856,7 +2860,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>24</v>
@@ -2910,7 +2914,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>24</v>
@@ -3001,7 +3005,7 @@
     <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>51</v>
@@ -3056,7 +3060,7 @@
         <v>26</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>24</v>
@@ -3109,7 +3113,7 @@
         <v>27</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>24</v>
@@ -3162,7 +3166,7 @@
         <v>28</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>24</v>
@@ -3213,7 +3217,7 @@
     <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>52</v>
@@ -3267,7 +3271,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>24</v>
@@ -3320,7 +3324,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>24</v>
@@ -3373,7 +3377,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>24</v>
@@ -3424,7 +3428,7 @@
     <row r="47" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>53</v>
@@ -3478,7 +3482,7 @@
         <v>32</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>24</v>
@@ -3531,7 +3535,7 @@
         <v>33</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>24</v>
@@ -3584,7 +3588,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>24</v>
@@ -3635,7 +3639,7 @@
     <row r="51" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>54</v>
@@ -3689,7 +3693,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>24</v>
@@ -3742,7 +3746,7 @@
         <v>36</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>24</v>
@@ -3795,7 +3799,7 @@
         <v>37</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>24</v>
@@ -3846,7 +3850,7 @@
     <row r="55" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>55</v>
@@ -3900,7 +3904,7 @@
         <v>38</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>24</v>
@@ -3953,7 +3957,7 @@
         <v>39</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>24</v>
@@ -4044,7 +4048,7 @@
     <row r="59" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>56</v>
@@ -4098,7 +4102,7 @@
         <v>40</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>24</v>
@@ -4151,7 +4155,7 @@
         <v>41</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>24</v>
@@ -4204,7 +4208,7 @@
         <v>42</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>24</v>
@@ -4255,7 +4259,7 @@
     <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>57</v>
@@ -4309,7 +4313,7 @@
         <v>43</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>24</v>
@@ -4362,7 +4366,7 @@
         <v>44</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>24</v>
@@ -4415,7 +4419,7 @@
         <v>45</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>24</v>
@@ -4466,7 +4470,7 @@
     <row r="67" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>58</v>
@@ -4520,7 +4524,7 @@
         <v>46</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>24</v>
@@ -4573,7 +4577,7 @@
         <v>47</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>24</v>
@@ -4598,7 +4602,9 @@
       </c>
     </row>
     <row r="70" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="7"/>
+      <c r="B70" s="7">
+        <v>48</v>
+      </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7" t="s">
         <v>24</v>
@@ -4617,7 +4623,7 @@
     <row r="71" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>59</v>
@@ -4647,7 +4653,7 @@
         <v>48</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>24</v>
@@ -4676,7 +4682,7 @@
         <v>49</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>24</v>
@@ -4705,7 +4711,7 @@
         <v>50</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>24</v>
@@ -4732,7 +4738,7 @@
     <row r="75" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>60</v>
@@ -4762,7 +4768,7 @@
         <v>51</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>24</v>
@@ -4791,7 +4797,7 @@
         <v>52</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>24</v>
@@ -4820,7 +4826,7 @@
         <v>53</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>24</v>
@@ -4847,7 +4853,7 @@
     <row r="79" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>61</v>
@@ -4859,7 +4865,7 @@
         <v>44010</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>7</v>
@@ -4877,7 +4883,7 @@
         <v>54</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>24</v>
@@ -4906,7 +4912,7 @@
         <v>55</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>24</v>
@@ -4918,7 +4924,7 @@
         <v>44012</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>7</v>
@@ -4950,10 +4956,10 @@
     <row r="83" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>24</v>
@@ -4980,7 +4986,7 @@
         <v>56</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>24</v>
@@ -5009,7 +5015,7 @@
         <v>57</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>24</v>
@@ -5053,10 +5059,10 @@
     <row r="87" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>24</v>
@@ -5083,7 +5089,7 @@
         <v>58</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>24</v>
@@ -5112,7 +5118,7 @@
         <v>59</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>24</v>
@@ -5141,7 +5147,7 @@
         <v>60</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>24</v>
@@ -5168,10 +5174,10 @@
     <row r="91" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>24</v>
@@ -5198,7 +5204,7 @@
         <v>61</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>24</v>
@@ -5260,7 +5266,7 @@
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>24</v>
@@ -5329,7 +5335,7 @@
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>24</v>
@@ -5398,7 +5404,7 @@
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>24</v>
@@ -5476,7 +5482,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Change project name from Sundew to Pitcher
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -27,11 +27,6 @@
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -41,7 +36,7 @@
     <author>Jordan</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0" shapeId="0">
+    <comment ref="B74" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +44,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Jordan:</t>
         </r>
@@ -58,11 +53,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Up to here.
-</t>
+Up to here!</t>
         </r>
       </text>
     </comment>
@@ -71,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="133">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -154,9 +148,6 @@
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
   </si>
   <si>
-    <t xml:space="preserve">SUNDEW - AGILE PRODUCT BACKLOG </t>
-  </si>
-  <si>
     <t>Redesign deployment portfolio</t>
   </si>
   <si>
@@ -467,6 +458,12 @@
   </si>
   <si>
     <t>Input sample data into app</t>
+  </si>
+  <si>
+    <t>2020/06/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PITCHER - AGILE PRODUCT BACKLOG </t>
   </si>
 </sst>
 </file>
@@ -540,14 +537,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -651,7 +648,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -700,6 +697,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1048,8 +1048,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
   <sheetData>
     <row r="1" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1165,13 +1165,13 @@
     <row r="3" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="6">
         <v>43871</v>
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>24</v>
@@ -1271,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>24</v>
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>24</v>
@@ -1385,7 +1385,7 @@
     <row r="7" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>1</v>
@@ -1442,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>24</v>
@@ -1491,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>24</v>
@@ -1543,7 +1543,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>24</v>
@@ -1593,7 +1593,7 @@
     <row r="11" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>2</v>
@@ -1646,7 +1646,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>24</v>
@@ -1698,7 +1698,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>24</v>
@@ -1750,7 +1750,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>24</v>
@@ -1800,7 +1800,7 @@
     <row r="15" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
@@ -1853,7 +1853,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>24</v>
@@ -1905,7 +1905,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>24</v>
@@ -1957,7 +1957,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>24</v>
@@ -2007,7 +2007,7 @@
     <row r="19" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>4</v>
@@ -2060,7 +2060,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>24</v>
@@ -2112,7 +2112,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>24</v>
@@ -2164,7 +2164,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>24</v>
@@ -2214,7 +2214,7 @@
     <row r="23" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>22</v>
@@ -2300,7 +2300,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>24</v>
@@ -2352,7 +2352,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>24</v>
@@ -2402,7 +2402,7 @@
     <row r="27" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
@@ -2489,7 +2489,7 @@
         <v>19</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>24</v>
@@ -2541,7 +2541,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>24</v>
@@ -2591,10 +2591,10 @@
     <row r="31" spans="2:35" s="12" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>24</v>
@@ -2645,7 +2645,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>24</v>
@@ -2699,7 +2699,7 @@
         <v>22</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
@@ -2753,7 +2753,7 @@
         <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>24</v>
@@ -2805,16 +2805,16 @@
     <row r="35" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F35" s="6">
-        <v>43886</v>
+        <v>43942</v>
       </c>
       <c r="G35" s="6">
         <v>43897</v>
@@ -2860,7 +2860,7 @@
         <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>24</v>
@@ -2869,10 +2869,10 @@
         <v>24</v>
       </c>
       <c r="F36" s="8">
-        <v>43887</v>
+        <v>43942</v>
       </c>
       <c r="G36" s="8">
-        <v>43890</v>
+        <v>43944</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>7</v>
@@ -2914,7 +2914,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>24</v>
@@ -2923,10 +2923,10 @@
         <v>24</v>
       </c>
       <c r="F37" s="8">
-        <v>43891</v>
+        <v>43945</v>
       </c>
       <c r="G37" s="8">
-        <v>43897</v>
+        <v>43948</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>7</v>
@@ -3005,19 +3005,19 @@
     <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F39" s="6">
-        <v>43898</v>
+        <v>43948</v>
       </c>
       <c r="G39" s="6">
-        <v>43913</v>
+        <v>43951</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>7</v>
@@ -3060,7 +3060,7 @@
         <v>26</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>24</v>
@@ -3069,10 +3069,10 @@
         <v>24</v>
       </c>
       <c r="F40" s="8">
-        <v>43898</v>
+        <v>43948</v>
       </c>
       <c r="G40" s="8">
-        <v>43905</v>
+        <v>43950</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>9</v>
@@ -3113,7 +3113,7 @@
         <v>27</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>24</v>
@@ -3122,7 +3122,7 @@
         <v>24</v>
       </c>
       <c r="F41" s="8">
-        <v>43906</v>
+        <v>43952</v>
       </c>
       <c r="G41" s="8">
         <v>43908</v>
@@ -3166,7 +3166,7 @@
         <v>28</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>24</v>
@@ -3217,10 +3217,10 @@
     <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>24</v>
@@ -3271,7 +3271,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>24</v>
@@ -3324,7 +3324,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>24</v>
@@ -3377,7 +3377,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>24</v>
@@ -3428,10 +3428,10 @@
     <row r="47" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>24</v>
@@ -3482,7 +3482,7 @@
         <v>32</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>24</v>
@@ -3535,7 +3535,7 @@
         <v>33</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>24</v>
@@ -3588,7 +3588,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>24</v>
@@ -3639,10 +3639,10 @@
     <row r="51" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>24</v>
@@ -3693,7 +3693,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>24</v>
@@ -3746,7 +3746,7 @@
         <v>36</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>24</v>
@@ -3799,7 +3799,7 @@
         <v>37</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>24</v>
@@ -3850,19 +3850,19 @@
     <row r="55" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F55" s="6">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="G55" s="6">
-        <v>43958</v>
+        <v>43954</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>7</v>
@@ -3904,7 +3904,7 @@
         <v>38</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>24</v>
@@ -3913,10 +3913,10 @@
         <v>24</v>
       </c>
       <c r="F56" s="8">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="G56" s="8">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>7</v>
@@ -3957,7 +3957,7 @@
         <v>39</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>24</v>
@@ -3966,10 +3966,10 @@
         <v>24</v>
       </c>
       <c r="F57" s="8">
-        <v>43953</v>
+        <v>43957</v>
       </c>
       <c r="G57" s="8">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>7</v>
@@ -4048,16 +4048,16 @@
     <row r="59" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F59" s="6">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="G59" s="6">
         <v>43965</v>
@@ -4102,7 +4102,7 @@
         <v>40</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>24</v>
@@ -4111,10 +4111,10 @@
         <v>24</v>
       </c>
       <c r="F60" s="8">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="G60" s="8">
-        <v>43961</v>
+        <v>43964</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>7</v>
@@ -4155,7 +4155,7 @@
         <v>41</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>24</v>
@@ -4164,10 +4164,10 @@
         <v>24</v>
       </c>
       <c r="F61" s="8">
-        <v>43962</v>
+        <v>43967</v>
       </c>
       <c r="G61" s="8">
-        <v>43963</v>
+        <v>43970</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>7</v>
@@ -4208,7 +4208,7 @@
         <v>42</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>24</v>
@@ -4217,10 +4217,10 @@
         <v>24</v>
       </c>
       <c r="F62" s="8">
-        <v>43964</v>
+        <v>43973</v>
       </c>
       <c r="G62" s="8">
-        <v>43965</v>
+        <v>43976</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>7</v>
@@ -4259,10 +4259,10 @@
     <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>24</v>
@@ -4313,7 +4313,7 @@
         <v>43</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>24</v>
@@ -4322,10 +4322,10 @@
         <v>24</v>
       </c>
       <c r="F64" s="8">
-        <v>43966</v>
+        <v>43976</v>
       </c>
       <c r="G64" s="8">
-        <v>43968</v>
+        <v>43979</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>8</v>
@@ -4366,7 +4366,7 @@
         <v>44</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>24</v>
@@ -4375,10 +4375,10 @@
         <v>24</v>
       </c>
       <c r="F65" s="8">
-        <v>43969</v>
+        <v>43981</v>
       </c>
       <c r="G65" s="8">
-        <v>43970</v>
+        <v>43985</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>8</v>
@@ -4419,7 +4419,7 @@
         <v>45</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>24</v>
@@ -4428,10 +4428,10 @@
         <v>24</v>
       </c>
       <c r="F66" s="8">
-        <v>43971</v>
+        <v>43988</v>
       </c>
       <c r="G66" s="8">
-        <v>43974</v>
+        <v>43991</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>7</v>
@@ -4470,19 +4470,19 @@
     <row r="67" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F67" s="6">
-        <v>43975</v>
-      </c>
-      <c r="G67" s="6">
-        <v>43981</v>
+        <v>43991</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>7</v>
@@ -4524,7 +4524,7 @@
         <v>46</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>24</v>
@@ -4533,10 +4533,10 @@
         <v>24</v>
       </c>
       <c r="F68" s="8">
-        <v>43975</v>
+        <v>43992</v>
       </c>
       <c r="G68" s="8">
-        <v>43978</v>
+        <v>43994</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>7</v>
@@ -4577,7 +4577,7 @@
         <v>47</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>24</v>
@@ -4586,10 +4586,10 @@
         <v>24</v>
       </c>
       <c r="F69" s="8">
-        <v>43979</v>
+        <v>43993</v>
       </c>
       <c r="G69" s="8">
-        <v>43981</v>
+        <v>43969</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>7</v>
@@ -4623,16 +4623,16 @@
     <row r="71" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F71" s="6">
-        <v>43982</v>
+        <v>43970</v>
       </c>
       <c r="G71" s="6">
         <v>43995</v>
@@ -4653,7 +4653,7 @@
         <v>48</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>24</v>
@@ -4662,10 +4662,10 @@
         <v>24</v>
       </c>
       <c r="F72" s="8">
-        <v>43982</v>
+        <v>43969</v>
       </c>
       <c r="G72" s="8">
-        <v>43986</v>
+        <v>44007</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>7</v>
@@ -4682,7 +4682,7 @@
         <v>49</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>24</v>
@@ -4691,10 +4691,10 @@
         <v>24</v>
       </c>
       <c r="F73" s="8">
-        <v>43987</v>
-      </c>
-      <c r="G73" s="8">
-        <v>43990</v>
+        <v>44010</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>7</v>
@@ -4711,7 +4711,7 @@
         <v>50</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>24</v>
@@ -4738,10 +4738,10 @@
     <row r="75" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>24</v>
@@ -4768,7 +4768,7 @@
         <v>51</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>24</v>
@@ -4797,7 +4797,7 @@
         <v>52</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>24</v>
@@ -4826,7 +4826,7 @@
         <v>53</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>24</v>
@@ -4853,10 +4853,10 @@
     <row r="79" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>24</v>
@@ -4865,7 +4865,7 @@
         <v>44010</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>7</v>
@@ -4883,7 +4883,7 @@
         <v>54</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>24</v>
@@ -4895,7 +4895,7 @@
         <v>44010</v>
       </c>
       <c r="G80" s="8">
-        <v>44011</v>
+        <v>44002</v>
       </c>
       <c r="H80" s="7" t="s">
         <v>7</v>
@@ -4912,7 +4912,7 @@
         <v>55</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>24</v>
@@ -4923,8 +4923,8 @@
       <c r="F81" s="8">
         <v>44012</v>
       </c>
-      <c r="G81" s="8" t="s">
-        <v>129</v>
+      <c r="G81" s="8">
+        <v>44014</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>7</v>
@@ -4956,16 +4956,16 @@
     <row r="83" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F83" s="6">
-        <v>43983</v>
+        <v>44016</v>
       </c>
       <c r="G83" s="6">
         <v>43989</v>
@@ -4986,7 +4986,7 @@
         <v>56</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>24</v>
@@ -4995,10 +4995,10 @@
         <v>24</v>
       </c>
       <c r="F84" s="8">
-        <v>43983</v>
+        <v>44016</v>
       </c>
       <c r="G84" s="8">
-        <v>43985</v>
+        <v>44017</v>
       </c>
       <c r="H84" s="7" t="s">
         <v>7</v>
@@ -5015,7 +5015,7 @@
         <v>57</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>24</v>
@@ -5024,10 +5024,10 @@
         <v>24</v>
       </c>
       <c r="F85" s="8">
-        <v>43987</v>
+        <v>44018</v>
       </c>
       <c r="G85" s="8">
-        <v>43989</v>
+        <v>44021</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>7</v>
@@ -5059,19 +5059,19 @@
     <row r="87" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F87" s="6">
-        <v>43990</v>
+        <v>44022</v>
       </c>
       <c r="G87" s="6">
-        <v>43998</v>
+        <v>43992</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>7</v>
@@ -5089,7 +5089,7 @@
         <v>58</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>24</v>
@@ -5098,10 +5098,10 @@
         <v>24</v>
       </c>
       <c r="F88" s="8">
-        <v>43990</v>
+        <v>44022</v>
       </c>
       <c r="G88" s="8">
-        <v>43992</v>
+        <v>44024</v>
       </c>
       <c r="H88" s="7" t="s">
         <v>7</v>
@@ -5118,7 +5118,7 @@
         <v>59</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>24</v>
@@ -5127,10 +5127,10 @@
         <v>24</v>
       </c>
       <c r="F89" s="8">
-        <v>43993</v>
+        <v>44025</v>
       </c>
       <c r="G89" s="8">
-        <v>43994</v>
+        <v>44027</v>
       </c>
       <c r="H89" s="7" t="s">
         <v>7</v>
@@ -5147,7 +5147,7 @@
         <v>60</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>24</v>
@@ -5156,10 +5156,10 @@
         <v>24</v>
       </c>
       <c r="F90" s="8">
-        <v>43995</v>
+        <v>44029</v>
       </c>
       <c r="G90" s="8">
-        <v>43998</v>
+        <v>44031</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>7</v>
@@ -5174,19 +5174,19 @@
     <row r="91" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F91" s="6">
-        <v>43998</v>
+        <v>44033</v>
       </c>
       <c r="G91" s="6">
-        <v>44000</v>
+        <v>44036</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>7</v>
@@ -5204,7 +5204,7 @@
         <v>61</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>24</v>
@@ -5212,11 +5212,11 @@
       <c r="E92" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F92" s="8">
-        <v>43998</v>
+      <c r="F92" s="20">
+        <v>44033</v>
       </c>
       <c r="G92" s="8">
-        <v>44000</v>
+        <v>44036</v>
       </c>
       <c r="H92" s="7" t="s">
         <v>7</v>
@@ -5266,7 +5266,7 @@
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>24</v>
@@ -5335,7 +5335,7 @@
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>24</v>
@@ -5404,7 +5404,7 @@
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>24</v>
@@ -5484,11 +5484,6 @@
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5518,10 +5513,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Up to task 3
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Sundew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1047,9 +1047,9 @@
   </sheetPr>
   <dimension ref="B1:AI106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
         <v>9</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J4" s="7">
         <v>2</v>
@@ -1289,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J5" s="7">
         <v>2</v>

</xml_diff>

<commit_message>
Up to task 6
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -27,7 +27,6 @@
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1049,8 +1048,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1183,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J3" s="5">
         <f>SUM(J4:J6)</f>
@@ -1461,7 +1460,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J8" s="7">
         <v>13</v>
@@ -1510,7 +1509,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J9" s="18">
         <v>1</v>
@@ -1562,7 +1561,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="7">
         <v>5</v>
@@ -1603,7 +1602,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="6">
-        <v>43883</v>
+        <v>43884</v>
       </c>
       <c r="G11" s="6">
         <v>43841</v>

</xml_diff>

<commit_message>
Up to task 12
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1048,8 +1048,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1561,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" s="7">
         <v>5</v>
@@ -1664,7 +1664,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J12" s="7">
         <v>13</v>
@@ -1697,8 +1697,8 @@
       <c r="B13" s="7">
         <v>8</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>31</v>
+      <c r="C13" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>24</v>
@@ -1716,7 +1716,7 @@
         <v>8</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J13" s="7">
         <v>5</v>
@@ -1750,7 +1750,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>24</v>
@@ -1768,7 +1768,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J14" s="7">
         <v>8</v>
@@ -1852,8 +1852,8 @@
       <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>33</v>
+      <c r="C16" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>24</v>
@@ -1876,7 +1876,6 @@
       <c r="J16" s="7">
         <v>1</v>
       </c>
-      <c r="K16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1905,7 +1904,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>24</v>
@@ -1928,7 +1927,6 @@
       <c r="J17" s="7">
         <v>8</v>
       </c>
-      <c r="K17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -1980,7 +1978,6 @@
       <c r="J18" s="7">
         <v>13</v>
       </c>
-      <c r="K18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>

</xml_diff>

<commit_message>
Cannot do task 11. Proceeding to 12
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426CA503-3744-4DF2-A990-0E514672C47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -26,17 +27,27 @@
     <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jordan</author>
   </authors>
   <commentList>
-    <comment ref="B74" authorId="0" shapeId="0">
+    <comment ref="B74" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -469,7 +480,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -704,7 +715,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1040,7 +1051,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1048,8 +1059,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1871,7 +1882,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J16" s="7">
         <v>1</v>
@@ -1922,7 +1933,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J17" s="7">
         <v>8</v>
@@ -1973,7 +1984,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J18" s="7">
         <v>13</v>
@@ -5468,13 +5479,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H106" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I106" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6">
+    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>$A$6:$A$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -5485,7 +5496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
Up to task 13
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426CA503-3744-4DF2-A990-0E514672C47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B57812-A6CC-4CFE-A701-523F8596DFDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="134">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t xml:space="preserve">PITCHER - AGILE PRODUCT BACKLOG </t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1062,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1152,9 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -1173,7 +1178,7 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>42</v>
@@ -1200,7 +1205,7 @@
         <f>SUM(J4:J6)</f>
         <v>17</v>
       </c>
-      <c r="K3" s="19"/>
+      <c r="K3" s="5"/>
       <c r="N3" s="3"/>
       <c r="P3"/>
       <c r="Q3"/>
@@ -1251,7 +1256,7 @@
       <c r="J4" s="7">
         <v>2</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="7"/>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
         <v>25</v>
@@ -1305,7 +1310,7 @@
       <c r="J5" s="7">
         <v>2</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="7"/>
       <c r="N5" s="3"/>
       <c r="O5" s="15" t="s">
         <v>5</v>
@@ -1363,7 +1368,7 @@
       <c r="J6" s="7">
         <v>13</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="7"/>
       <c r="N6" s="3"/>
       <c r="O6" s="15" t="s">
         <v>6</v>
@@ -1414,13 +1419,13 @@
         <v>7</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J7" s="5">
         <f>SUM(J8:J10)</f>
         <v>19</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="5"/>
       <c r="N7" s="3"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15" t="s">
@@ -1476,7 +1481,7 @@
       <c r="J8" s="7">
         <v>13</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="7"/>
       <c r="N8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -1525,7 +1530,7 @@
       <c r="J9" s="18">
         <v>1</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="18"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1577,7 +1582,7 @@
       <c r="J10" s="7">
         <v>5</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="7"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -1622,13 +1627,13 @@
         <v>8</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J11" s="5">
         <f>SUM(J12:J14)</f>
         <v>26</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="5"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -1680,7 +1685,7 @@
       <c r="J12" s="7">
         <v>13</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="7"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -1732,7 +1737,7 @@
       <c r="J13" s="7">
         <v>5</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="7"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -1784,7 +1789,7 @@
       <c r="J14" s="7">
         <v>8</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="7"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -1829,13 +1834,13 @@
         <v>7</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J15" s="5">
         <f>SUM(J16:J18)</f>
         <v>22</v>
       </c>
-      <c r="K15" s="3"/>
+      <c r="K15" s="5"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -1887,6 +1892,7 @@
       <c r="J16" s="7">
         <v>1</v>
       </c>
+      <c r="K16" s="7"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1938,6 +1944,7 @@
       <c r="J17" s="7">
         <v>8</v>
       </c>
+      <c r="K17" s="7"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -1989,6 +1996,7 @@
       <c r="J18" s="7">
         <v>13</v>
       </c>
+      <c r="K18" s="7"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -2039,7 +2047,7 @@
         <f>SUM(J20:J22)</f>
         <v>100</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="5"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -2086,12 +2094,12 @@
         <v>8</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J20" s="7">
         <v>20</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="7"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -2138,12 +2146,12 @@
         <v>7</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21" s="7">
         <v>40</v>
       </c>
-      <c r="K21" s="3"/>
+      <c r="K21" s="7"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -2190,12 +2198,12 @@
         <v>7</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J22" s="7">
         <v>40</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="7"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -2246,7 +2254,7 @@
         <f>SUM(J24:J26)</f>
         <v>80</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="5"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -2279,7 +2287,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="3"/>
+      <c r="K24" s="7"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -2326,12 +2334,12 @@
         <v>7</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J25" s="7">
         <v>40</v>
       </c>
-      <c r="K25" s="3"/>
+      <c r="K25" s="7"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -2378,12 +2386,12 @@
         <v>7</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J26" s="7">
         <v>40</v>
       </c>
-      <c r="K26" s="3"/>
+      <c r="K26" s="7"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -2434,7 +2442,7 @@
         <f>SUM(J28:J30)</f>
         <v>80</v>
       </c>
-      <c r="K27" s="3"/>
+      <c r="K27" s="5"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -2468,7 +2476,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="3"/>
+      <c r="K28" s="7"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -2520,7 +2528,7 @@
       <c r="J29" s="7">
         <v>40</v>
       </c>
-      <c r="K29" s="3"/>
+      <c r="K29" s="7"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -2572,7 +2580,7 @@
       <c r="J30" s="7">
         <v>40</v>
       </c>
-      <c r="K30" s="3"/>
+      <c r="K30" s="7"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -2623,7 +2631,7 @@
         <f>SUM(J32:J34)</f>
         <v>47</v>
       </c>
-      <c r="K31" s="19"/>
+      <c r="K31" s="5"/>
       <c r="L31" s="19"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -2671,12 +2679,12 @@
         <v>9</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J32" s="7">
         <v>2</v>
       </c>
-      <c r="K32" s="3"/>
+      <c r="K32" s="7"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
@@ -2725,12 +2733,12 @@
         <v>8</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J33" s="7">
         <v>5</v>
       </c>
-      <c r="K33" s="3"/>
+      <c r="K33" s="7"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -2779,12 +2787,12 @@
         <v>7</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J34" s="7">
         <v>40</v>
       </c>
-      <c r="K34" s="3"/>
+      <c r="K34" s="7"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -2837,7 +2845,7 @@
         <f>SUM(J36:J38)</f>
         <v>80</v>
       </c>
-      <c r="K35" s="3"/>
+      <c r="K35" s="5"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -2886,12 +2894,12 @@
         <v>7</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J36" s="7">
         <v>40</v>
       </c>
-      <c r="K36" s="3"/>
+      <c r="K36" s="7"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -2945,7 +2953,7 @@
       <c r="J37" s="7">
         <v>40</v>
       </c>
-      <c r="K37" s="3"/>
+      <c r="K37" s="7"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -2984,7 +2992,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
-      <c r="K38" s="3"/>
+      <c r="K38" s="7"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -3037,7 +3045,7 @@
         <f>SUM(J40:J42)</f>
         <v>81</v>
       </c>
-      <c r="K39" s="3"/>
+      <c r="K39" s="5"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -3091,6 +3099,7 @@
       <c r="J40" s="7">
         <v>1</v>
       </c>
+      <c r="K40" s="7"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -3144,6 +3153,7 @@
       <c r="J41" s="7">
         <v>40</v>
       </c>
+      <c r="K41" s="7"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -3197,6 +3207,7 @@
       <c r="J42" s="7">
         <v>40</v>
       </c>
+      <c r="K42" s="7"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -3249,6 +3260,7 @@
         <f>SUM(J44:J46)</f>
         <v>38</v>
       </c>
+      <c r="K43" s="5"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -3302,6 +3314,7 @@
       <c r="J44" s="7">
         <v>13</v>
       </c>
+      <c r="K44" s="7"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -3355,6 +3368,7 @@
       <c r="J45" s="7">
         <v>5</v>
       </c>
+      <c r="K45" s="7"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -3408,6 +3422,7 @@
       <c r="J46" s="7">
         <v>20</v>
       </c>
+      <c r="K46" s="7"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -3460,6 +3475,7 @@
         <f>SUM(J48:J50)</f>
         <v>100</v>
       </c>
+      <c r="K47" s="5"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -3513,6 +3529,7 @@
       <c r="J48" s="7">
         <v>40</v>
       </c>
+      <c r="K48" s="7"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -3566,6 +3583,7 @@
       <c r="J49" s="7">
         <v>40</v>
       </c>
+      <c r="K49" s="7"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3619,6 +3637,7 @@
       <c r="J50" s="7">
         <v>20</v>
       </c>
+      <c r="K50" s="7"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -3671,6 +3690,7 @@
         <f>SUM(J52:J54)</f>
         <v>38</v>
       </c>
+      <c r="K51" s="5"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -3724,6 +3744,7 @@
       <c r="J52" s="7">
         <v>5</v>
       </c>
+      <c r="K52" s="7"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
@@ -3777,6 +3798,7 @@
       <c r="J53" s="7">
         <v>13</v>
       </c>
+      <c r="K53" s="7"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
@@ -3830,6 +3852,7 @@
       <c r="J54" s="7">
         <v>20</v>
       </c>
+      <c r="K54" s="7"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
@@ -3882,6 +3905,7 @@
         <f>SUM(J56:J58)</f>
         <v>80</v>
       </c>
+      <c r="K55" s="5"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -3935,6 +3959,7 @@
       <c r="J56" s="7">
         <v>40</v>
       </c>
+      <c r="K56" s="7"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
@@ -3988,6 +4013,7 @@
       <c r="J57" s="7">
         <v>40</v>
       </c>
+      <c r="K57" s="7"/>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
@@ -4028,6 +4054,7 @@
         <v>12</v>
       </c>
       <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
@@ -4080,6 +4107,7 @@
         <f>SUM(J60:J62)</f>
         <v>120</v>
       </c>
+      <c r="K59" s="5"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
@@ -4133,6 +4161,7 @@
       <c r="J60" s="7">
         <v>40</v>
       </c>
+      <c r="K60" s="7"/>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
@@ -4186,6 +4215,7 @@
       <c r="J61" s="7">
         <v>40</v>
       </c>
+      <c r="K61" s="7"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
@@ -4239,6 +4269,7 @@
       <c r="J62" s="7">
         <v>40</v>
       </c>
+      <c r="K62" s="7"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
@@ -4291,6 +4322,7 @@
         <f>SUM(J64:J66)</f>
         <v>39</v>
       </c>
+      <c r="K63" s="5"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
@@ -4344,6 +4376,7 @@
       <c r="J64" s="7">
         <v>13</v>
       </c>
+      <c r="K64" s="7"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
@@ -4397,6 +4430,7 @@
       <c r="J65" s="7">
         <v>13</v>
       </c>
+      <c r="K65" s="7"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
@@ -4450,6 +4484,7 @@
       <c r="J66" s="7">
         <v>13</v>
       </c>
+      <c r="K66" s="7"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
@@ -4502,6 +4537,7 @@
         <f>SUM(J68:J70)</f>
         <v>80</v>
       </c>
+      <c r="K67" s="5"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
@@ -4555,6 +4591,7 @@
       <c r="J68" s="7">
         <v>40</v>
       </c>
+      <c r="K68" s="7"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
@@ -4608,6 +4645,7 @@
       <c r="J69" s="7">
         <v>40</v>
       </c>
+      <c r="K69" s="7"/>
     </row>
     <row r="70" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
@@ -4627,6 +4665,7 @@
         <v>12</v>
       </c>
       <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
     </row>
     <row r="71" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
@@ -4655,6 +4694,7 @@
         <f>SUM(J72:J74)</f>
         <v>120</v>
       </c>
+      <c r="K71" s="5"/>
     </row>
     <row r="72" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
@@ -4684,6 +4724,7 @@
       <c r="J72" s="7">
         <v>40</v>
       </c>
+      <c r="K72" s="7"/>
     </row>
     <row r="73" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="7">
@@ -4713,6 +4754,7 @@
       <c r="J73" s="7">
         <v>40</v>
       </c>
+      <c r="K73" s="7"/>
     </row>
     <row r="74" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="7">
@@ -4742,6 +4784,7 @@
       <c r="J74" s="7">
         <v>40</v>
       </c>
+      <c r="K74" s="7"/>
     </row>
     <row r="75" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
@@ -4770,6 +4813,7 @@
         <f>SUM(J76:J78)</f>
         <v>101</v>
       </c>
+      <c r="K75" s="5"/>
     </row>
     <row r="76" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="7">
@@ -4799,6 +4843,7 @@
       <c r="J76" s="7">
         <v>40</v>
       </c>
+      <c r="K76" s="7"/>
     </row>
     <row r="77" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="7">
@@ -4828,6 +4873,7 @@
       <c r="J77" s="7">
         <v>21</v>
       </c>
+      <c r="K77" s="7"/>
     </row>
     <row r="78" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="7">
@@ -4857,6 +4903,7 @@
       <c r="J78" s="7">
         <v>40</v>
       </c>
+      <c r="K78" s="7"/>
     </row>
     <row r="79" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
@@ -4885,6 +4932,7 @@
         <f>SUM(J80:J82)</f>
         <v>53</v>
       </c>
+      <c r="K79" s="5"/>
     </row>
     <row r="80" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="7">
@@ -4914,8 +4962,9 @@
       <c r="J80" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K80" s="7"/>
+    </row>
+    <row r="81" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="7">
         <v>55</v>
       </c>
@@ -4943,8 +4992,9 @@
       <c r="J81" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="82" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K81" s="7"/>
+    </row>
+    <row r="82" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7" t="s">
@@ -4960,8 +5010,9 @@
         <v>12</v>
       </c>
       <c r="J82" s="7"/>
-    </row>
-    <row r="83" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K82" s="7"/>
+    </row>
+    <row r="83" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
         <v>121</v>
@@ -4988,8 +5039,9 @@
         <f>SUM(J84:J86)</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K83" s="5"/>
+    </row>
+    <row r="84" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="7">
         <v>56</v>
       </c>
@@ -5017,8 +5069,9 @@
       <c r="J84" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="85" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K84" s="7"/>
+    </row>
+    <row r="85" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="7">
         <v>57</v>
       </c>
@@ -5046,8 +5099,9 @@
       <c r="J85" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="86" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K85" s="7"/>
+    </row>
+    <row r="86" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7" t="s">
@@ -5063,8 +5117,9 @@
         <v>12</v>
       </c>
       <c r="J86" s="7"/>
-    </row>
-    <row r="87" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K86" s="7"/>
+    </row>
+    <row r="87" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
         <v>126</v>
@@ -5091,8 +5146,9 @@
         <f>SUM(J88:J90)</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="88" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="7">
         <v>58</v>
       </c>
@@ -5120,8 +5176,9 @@
       <c r="J88" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="89" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K88" s="7"/>
+    </row>
+    <row r="89" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="7">
         <v>59</v>
       </c>
@@ -5149,8 +5206,9 @@
       <c r="J89" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="90" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K89" s="7"/>
+    </row>
+    <row r="90" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="7">
         <v>60</v>
       </c>
@@ -5178,8 +5236,9 @@
       <c r="J90" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="91" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
         <v>122</v>
@@ -5206,8 +5265,9 @@
         <f>SUM(J92:J94)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="92" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="7">
         <v>61</v>
       </c>
@@ -5235,8 +5295,9 @@
       <c r="J92" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="93" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7" t="s">
@@ -5252,8 +5313,9 @@
         <v>12</v>
       </c>
       <c r="J93" s="7"/>
-    </row>
-    <row r="94" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K93" s="7"/>
+    </row>
+    <row r="94" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7" t="s">
@@ -5269,8 +5331,9 @@
         <v>12</v>
       </c>
       <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K94" s="7"/>
+    </row>
+    <row r="95" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5" t="s">
@@ -5287,8 +5350,9 @@
         <f>SUM(J96:J98)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
@@ -5304,8 +5368,9 @@
         <v>12</v>
       </c>
       <c r="J96" s="7"/>
-    </row>
-    <row r="97" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K96" s="7"/>
+    </row>
+    <row r="97" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7" t="s">
@@ -5321,8 +5386,9 @@
         <v>12</v>
       </c>
       <c r="J97" s="7"/>
-    </row>
-    <row r="98" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7" t="s">
@@ -5338,8 +5404,9 @@
         <v>12</v>
       </c>
       <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K98" s="7"/>
+    </row>
+    <row r="99" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5" t="s">
@@ -5356,8 +5423,9 @@
         <f>SUM(J100:J102)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
@@ -5373,8 +5441,9 @@
         <v>12</v>
       </c>
       <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K100" s="7"/>
+    </row>
+    <row r="101" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7" t="s">
@@ -5390,8 +5459,9 @@
         <v>12</v>
       </c>
       <c r="J101" s="7"/>
-    </row>
-    <row r="102" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K101" s="7"/>
+    </row>
+    <row r="102" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7" t="s">
@@ -5407,8 +5477,9 @@
         <v>12</v>
       </c>
       <c r="J102" s="7"/>
-    </row>
-    <row r="103" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K102" s="7"/>
+    </row>
+    <row r="103" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5" t="s">
@@ -5425,8 +5496,9 @@
         <f>SUM(J104:J106)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K103" s="5"/>
+    </row>
+    <row r="104" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7" t="s">
@@ -5442,8 +5514,9 @@
         <v>12</v>
       </c>
       <c r="J104" s="7"/>
-    </row>
-    <row r="105" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7" t="s">
@@ -5459,8 +5532,9 @@
         <v>12</v>
       </c>
       <c r="J105" s="7"/>
-    </row>
-    <row r="106" spans="2:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7" t="s">
@@ -5476,6 +5550,7 @@
         <v>12</v>
       </c>
       <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>

<commit_message>
Up to task 14
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E89BFE-20C4-4F91-8BF0-4738A8CFE1D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21CA6E6-95AF-4AFC-BB70-19F522863778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25290" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1062,8 +1062,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2146,7 @@
         <v>7</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J21" s="7">
         <v>40</v>
@@ -2198,7 +2198,7 @@
         <v>7</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J22" s="7">
         <v>40</v>

</xml_diff>

<commit_message>
Up to task 60
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21CA6E6-95AF-4AFC-BB70-19F522863778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1EFB70-1A32-411A-BC38-EA10B00BAD6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25290" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14430" yWindow="1710" windowWidth="25290" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="136">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -478,13 +478,19 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Aborted.</t>
+  </si>
+  <si>
+    <t>Decided to manually implement job start.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -560,8 +566,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,6 +595,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,7 +680,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -712,6 +730,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1061,9 +1088,9 @@
   </sheetPr>
   <dimension ref="B1:AI106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1104,7 @@
     <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="13.75" style="4" customWidth="1"/>
     <col min="10" max="10" width="15.25" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.75" style="4" customWidth="1"/>
+    <col min="11" max="11" width="31.375" style="4" customWidth="1"/>
     <col min="12" max="12" width="13.75" style="4" customWidth="1"/>
     <col min="13" max="13" width="11.25" style="4" customWidth="1"/>
     <col min="14" max="14" width="3.25" style="4" customWidth="1"/>
@@ -1814,33 +1841,33 @@
       <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="E15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="23">
         <v>43891</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="23">
         <v>43896</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="5">
+      <c r="H15" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="22">
         <f>SUM(J16:J18)</f>
         <v>22</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="22"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -2041,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J19" s="5">
         <f>SUM(J20:J22)</f>
@@ -2198,7 +2225,7 @@
         <v>7</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J22" s="7">
         <v>40</v>
@@ -2248,7 +2275,7 @@
         <v>8</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J23" s="5">
         <f>SUM(J24:J26)</f>
@@ -2436,7 +2463,7 @@
         <v>7</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J27" s="5">
         <f>SUM(J28:J30)</f>
@@ -2523,7 +2550,7 @@
         <v>7</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J29" s="7">
         <v>40</v>
@@ -2575,7 +2602,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J30" s="7">
         <v>40</v>
@@ -2625,7 +2652,7 @@
         <v>9</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J31" s="5">
         <f>SUM(J32:J34)</f>
@@ -2839,7 +2866,7 @@
         <v>7</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J35" s="5">
         <f>SUM(J36:J38)</f>
@@ -2948,7 +2975,7 @@
         <v>7</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J37" s="7">
         <v>40</v>
@@ -3039,7 +3066,7 @@
         <v>7</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J39" s="5">
         <f>SUM(J40:J42)</f>
@@ -3094,7 +3121,7 @@
         <v>9</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J40" s="7">
         <v>1</v>
@@ -3148,7 +3175,7 @@
         <v>7</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J41" s="7">
         <v>40</v>
@@ -3202,7 +3229,7 @@
         <v>7</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J42" s="7">
         <v>40</v>
@@ -3254,7 +3281,7 @@
         <v>8</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J43" s="5">
         <f>SUM(J44:J46)</f>
@@ -3309,7 +3336,7 @@
         <v>7</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J44" s="7">
         <v>13</v>
@@ -3363,7 +3390,7 @@
         <v>8</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J45" s="7">
         <v>5</v>
@@ -3417,12 +3444,14 @@
         <v>7</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J46" s="7">
         <v>20</v>
       </c>
-      <c r="K46" s="7"/>
+      <c r="K46" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -3469,7 +3498,7 @@
         <v>7</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J47" s="5">
         <f>SUM(J48:J50)</f>
@@ -3524,12 +3553,14 @@
         <v>7</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J48" s="7">
         <v>40</v>
       </c>
-      <c r="K48" s="7"/>
+      <c r="K48" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -3578,7 +3609,7 @@
         <v>7</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J49" s="7">
         <v>40</v>
@@ -3632,7 +3663,7 @@
         <v>7</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J50" s="7">
         <v>20</v>
@@ -3684,7 +3715,7 @@
         <v>8</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J51" s="5">
         <f>SUM(J52:J54)</f>
@@ -3739,7 +3770,7 @@
         <v>9</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J52" s="7">
         <v>5</v>
@@ -3793,7 +3824,7 @@
         <v>7</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J53" s="7">
         <v>13</v>
@@ -3847,12 +3878,14 @@
         <v>7</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J54" s="7">
         <v>20</v>
       </c>
-      <c r="K54" s="7"/>
+      <c r="K54" s="7" t="s">
+        <v>135</v>
+      </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
@@ -3899,7 +3932,7 @@
         <v>7</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J55" s="5">
         <f>SUM(J56:J58)</f>
@@ -3954,7 +3987,7 @@
         <v>7</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J56" s="7">
         <v>40</v>
@@ -4008,7 +4041,7 @@
         <v>7</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J57" s="7">
         <v>40</v>
@@ -4050,9 +4083,7 @@
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="7"/>
-      <c r="I58" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
       <c r="L58" s="3"/>
@@ -4101,7 +4132,7 @@
         <v>7</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J59" s="5">
         <f>SUM(J60:J62)</f>
@@ -4155,7 +4186,7 @@
       <c r="H60" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I60" s="21" t="s">
         <v>12</v>
       </c>
       <c r="J60" s="7">
@@ -4242,31 +4273,31 @@
       <c r="AI61" s="3"/>
     </row>
     <row r="62" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="7">
+      <c r="B62" s="18">
         <v>42</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F62" s="8">
+      <c r="D62" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="20">
         <v>43973</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="20">
         <v>43976</v>
       </c>
-      <c r="H62" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I62" s="7" t="s">
+      <c r="H62" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J62" s="7">
+      <c r="J62" s="18">
         <v>40</v>
       </c>
       <c r="K62" s="7"/>

</xml_diff>

<commit_message>
Almost 3 quater of a way through. Complete task 42
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Nash\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1EFB70-1A32-411A-BC38-EA10B00BAD6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82DF881-9F56-4CFF-A508-492E14F8FAC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14430" yWindow="1710" windowWidth="25290" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -41,42 +41,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Jordan</author>
-  </authors>
-  <commentList>
-    <comment ref="B74" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Jordan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Up to here!</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="137">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -483,14 +449,17 @@
     <t>Aborted.</t>
   </si>
   <si>
-    <t>Decided to manually implement job start.</t>
+    <t>Decided to manually implement job start. No automation.</t>
+  </si>
+  <si>
+    <t>Decided to not implement feature. Not needed right now.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,19 +521,6 @@
       <color theme="0"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -732,7 +688,7 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,16 +1037,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AI106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4187,12 +4143,14 @@
         <v>7</v>
       </c>
       <c r="I60" s="21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J60" s="7">
         <v>40</v>
       </c>
-      <c r="K60" s="7"/>
+      <c r="K60" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
@@ -4219,34 +4177,34 @@
       <c r="AI60" s="3"/>
     </row>
     <row r="61" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="7">
+      <c r="B61" s="22">
         <v>41</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="8">
+      <c r="D61" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="23">
         <v>43967</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="23">
         <v>43970</v>
       </c>
-      <c r="H61" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J61" s="7">
+      <c r="H61" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" s="22">
         <v>40</v>
       </c>
-      <c r="K61" s="7"/>
+      <c r="K61" s="22"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
@@ -4295,7 +4253,7 @@
         <v>7</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J62" s="18">
         <v>40</v>
@@ -4402,7 +4360,7 @@
         <v>8</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J64" s="7">
         <v>13</v>
@@ -4456,12 +4414,14 @@
         <v>8</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J65" s="7">
         <v>13</v>
       </c>
-      <c r="K65" s="7"/>
+      <c r="K65" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
@@ -4510,12 +4470,14 @@
         <v>7</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J66" s="7">
         <v>13</v>
       </c>
-      <c r="K66" s="7"/>
+      <c r="K66" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
@@ -4617,7 +4579,7 @@
         <v>7</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J68" s="7">
         <v>40</v>
@@ -5597,7 +5559,6 @@
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add empty header to resolve joined Problem actions Details, Edit, Delete
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CA1BBD-C665-4B73-87AE-4D637801EE1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C728551-6509-48F3-88A2-39C0F86ECAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,6 @@
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="137">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -1045,9 +1044,9 @@
   </sheetPr>
   <dimension ref="B1:AI106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4178,34 +4177,34 @@
       <c r="AI60" s="3"/>
     </row>
     <row r="61" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="22">
+      <c r="B61" s="18">
         <v>41</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="23">
+      <c r="D61" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="20">
         <v>43967</v>
       </c>
-      <c r="G61" s="23">
+      <c r="G61" s="20">
         <v>43970</v>
       </c>
-      <c r="H61" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J61" s="22">
+      <c r="H61" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J61" s="18">
         <v>40</v>
       </c>
-      <c r="K61" s="22"/>
+      <c r="K61" s="18"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
@@ -5299,9 +5298,7 @@
       <c r="F93" s="8"/>
       <c r="G93" s="8"/>
       <c r="H93" s="7"/>
-      <c r="I93" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I93" s="7"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
     </row>
@@ -5317,9 +5314,7 @@
       <c r="F94" s="8"/>
       <c r="G94" s="8"/>
       <c r="H94" s="7"/>
-      <c r="I94" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I94" s="7"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
     </row>
@@ -5354,9 +5349,7 @@
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="7"/>
-      <c r="I96" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I96" s="7"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
     </row>
@@ -5372,9 +5365,7 @@
       <c r="F97" s="8"/>
       <c r="G97" s="8"/>
       <c r="H97" s="7"/>
-      <c r="I97" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I97" s="7"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
     </row>
@@ -5390,9 +5381,7 @@
       <c r="F98" s="8"/>
       <c r="G98" s="8"/>
       <c r="H98" s="7"/>
-      <c r="I98" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
     </row>
@@ -5427,9 +5416,7 @@
       <c r="F100" s="8"/>
       <c r="G100" s="8"/>
       <c r="H100" s="7"/>
-      <c r="I100" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
     </row>
@@ -5445,9 +5432,7 @@
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
       <c r="H101" s="7"/>
-      <c r="I101" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
     </row>
@@ -5463,9 +5448,7 @@
       <c r="F102" s="8"/>
       <c r="G102" s="8"/>
       <c r="H102" s="7"/>
-      <c r="I102" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
     </row>
@@ -5500,9 +5483,7 @@
       <c r="F104" s="8"/>
       <c r="G104" s="8"/>
       <c r="H104" s="7"/>
-      <c r="I104" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I104" s="7"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
     </row>
@@ -5518,9 +5499,7 @@
       <c r="F105" s="8"/>
       <c r="G105" s="8"/>
       <c r="H105" s="7"/>
-      <c r="I105" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I105" s="7"/>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
@@ -5536,9 +5515,7 @@
       <c r="F106" s="8"/>
       <c r="G106" s="8"/>
       <c r="H106" s="7"/>
-      <c r="I106" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I106" s="7"/>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
     </row>

</xml_diff>

<commit_message>
Finish task 34, now at task 41
</commit_message>
<xml_diff>
--- a/Agile-Product-Backlog.xlsx
+++ b/Agile-Product-Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C728551-6509-48F3-88A2-39C0F86ECAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380816C2-18DE-446A-9482-9A9FBC3081AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2595" windowWidth="2400" windowHeight="585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -527,6 +527,11 @@
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -636,7 +641,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -695,6 +700,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1044,9 +1055,9 @@
   </sheetPr>
   <dimension ref="B1:AI106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3597,34 +3608,34 @@
       <c r="AI49" s="3"/>
     </row>
     <row r="50" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="22">
+      <c r="B50" s="24">
         <v>34</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="23">
+      <c r="D50" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="25">
         <v>43938</v>
       </c>
-      <c r="G50" s="23">
-        <v>43941</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J50" s="22">
+      <c r="G50" s="25">
+        <v>44094</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="24">
         <v>20</v>
       </c>
-      <c r="K50" s="22"/>
+      <c r="K50" s="24"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -4177,34 +4188,34 @@
       <c r="AI60" s="3"/>
     </row>
     <row r="61" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="18">
+      <c r="B61" s="22">
         <v>41</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C61" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="20">
+      <c r="D61" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="23">
         <v>43967</v>
       </c>
-      <c r="G61" s="20">
+      <c r="G61" s="23">
         <v>43970</v>
       </c>
-      <c r="H61" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J61" s="18">
+      <c r="H61" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" s="22">
         <v>40</v>
       </c>
-      <c r="K61" s="18"/>
+      <c r="K61" s="22"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>

</xml_diff>